<commit_message>
- another readme improvement - removed possible division by 0
</commit_message>
<xml_diff>
--- a/data/hsr/out.xlsx
+++ b/data/hsr/out.xlsx
@@ -1096,27 +1096,27 @@
         <v>17</v>
       </c>
       <c r="C28" s="6">
-        <f>SUM(C29:C34)/SUM(I29:I34)</f>
+        <f>IF(SUM(I29:I34)=0,0,(SUM(C29:C34)/SUM(I29:I34))</f>
         <v/>
       </c>
       <c r="D28" s="6">
-        <f>SUM(D29:D34)/SUM(I29:I34)</f>
+        <f>IF(SUM(I29:I34)=0,0,(SUM(D29:D34)/SUM(I29:I34))</f>
         <v/>
       </c>
       <c r="E28" s="6">
-        <f>SUM(E29:E34)/SUM(I29:I34)</f>
+        <f>IF(SUM(I29:I34)=0,0,(SUM(E29:E34)/SUM(I29:I34))</f>
         <v/>
       </c>
       <c r="F28" s="6">
-        <f>SUM(F29:F34)/SUM(I29:I34)</f>
+        <f>IF(SUM(I29:I34)=0,0,(SUM(F29:F34)/SUM(I29:I34))</f>
         <v/>
       </c>
       <c r="G28" s="6">
-        <f>SUM(G29:G34)/SUM(I29:I34)</f>
+        <f>IF(SUM(I29:I34)=0,0,(SUM(G29:G34)/SUM(I29:I34))</f>
         <v/>
       </c>
       <c r="H28" s="6">
-        <f>SUM(H29:H34)/SUM(I29:I34)</f>
+        <f>IF(SUM(I29:I34)=0,0,(SUM(H29:H34)/SUM(I29:I34))</f>
         <v/>
       </c>
     </row>
@@ -1349,15 +1349,15 @@
         <v>17</v>
       </c>
       <c r="C37" s="6">
-        <f>SUM(C38:C43)/SUM(F38:F43)</f>
+        <f>IF(SUM(F38:F43)=0,0,(SUM(C38:C43)/SUM(F38:F43))</f>
         <v/>
       </c>
       <c r="D37" s="6">
-        <f>SUM(D38:D43)/SUM(F38:F43)</f>
+        <f>IF(SUM(F38:F43)=0,0,(SUM(D38:D43)/SUM(F38:F43))</f>
         <v/>
       </c>
       <c r="E37" s="6">
-        <f>SUM(E38:E43)/SUM(F38:F43)</f>
+        <f>IF(SUM(F38:F43)=0,0,(SUM(E38:E43)/SUM(F38:F43))</f>
         <v/>
       </c>
     </row>
@@ -1520,11 +1520,11 @@
         <v>17</v>
       </c>
       <c r="C46" s="6">
-        <f>SUM(C47:C52)/SUM(E47:E52)</f>
+        <f>IF(SUM(E47:E52)=0,0,(SUM(C47:C52)/SUM(E47:E52))</f>
         <v/>
       </c>
       <c r="D46" s="6">
-        <f>SUM(D47:D52)/SUM(E47:E52)</f>
+        <f>IF(SUM(E47:E52)=0,0,(SUM(D47:D52)/SUM(E47:E52))</f>
         <v/>
       </c>
     </row>
@@ -1687,31 +1687,31 @@
         <v>17</v>
       </c>
       <c r="C61" s="6">
-        <f>SUM(C62:C64)/SUM(J62:J64)</f>
+        <f>IF(SUM(J62:J64)=0,0,(SUM(C62:C64)/SUM(J62:J64))</f>
         <v/>
       </c>
       <c r="D61" s="6">
-        <f>SUM(D62:D64)/SUM(J62:J64)</f>
+        <f>IF(SUM(J62:J64)=0,0,(SUM(D62:D64)/SUM(J62:J64))</f>
         <v/>
       </c>
       <c r="E61" s="6">
-        <f>SUM(E62:E64)/SUM(J62:J64)</f>
+        <f>IF(SUM(J62:J64)=0,0,(SUM(E62:E64)/SUM(J62:J64))</f>
         <v/>
       </c>
       <c r="F61" s="6">
-        <f>SUM(F62:F64)/SUM(J62:J64)</f>
+        <f>IF(SUM(J62:J64)=0,0,(SUM(F62:F64)/SUM(J62:J64))</f>
         <v/>
       </c>
       <c r="G61" s="6">
-        <f>SUM(G62:G64)/SUM(J62:J64)</f>
+        <f>IF(SUM(J62:J64)=0,0,(SUM(G62:G64)/SUM(J62:J64))</f>
         <v/>
       </c>
       <c r="H61" s="6">
-        <f>SUM(H62:H64)/SUM(J62:J64)</f>
+        <f>IF(SUM(J62:J64)=0,0,(SUM(H62:H64)/SUM(J62:J64))</f>
         <v/>
       </c>
       <c r="I61" s="6">
-        <f>SUM(I62:I64)/SUM(J62:J64)</f>
+        <f>IF(SUM(J62:J64)=0,0,(SUM(I62:I64)/SUM(J62:J64))</f>
         <v/>
       </c>
     </row>
@@ -1850,11 +1850,11 @@
         <v>17</v>
       </c>
       <c r="C67" s="6">
-        <f>SUM(C68:C70)/SUM(E68:E70)</f>
+        <f>IF(SUM(E68:E70)=0,0,(SUM(C68:C70)/SUM(E68:E70))</f>
         <v/>
       </c>
       <c r="D67" s="6">
-        <f>SUM(D68:D70)/SUM(E68:E70)</f>
+        <f>IF(SUM(E68:E70)=0,0,(SUM(D68:D70)/SUM(E68:E70))</f>
         <v/>
       </c>
     </row>
@@ -1938,11 +1938,11 @@
         <v>17</v>
       </c>
       <c r="C73" s="6">
-        <f>SUM(C74:C76)/SUM(E74:E76)</f>
+        <f>IF(SUM(E74:E76)=0,0,(SUM(C74:C76)/SUM(E74:E76))</f>
         <v/>
       </c>
       <c r="D73" s="6">
-        <f>SUM(D74:D76)/SUM(E74:E76)</f>
+        <f>IF(SUM(E74:E76)=0,0,(SUM(D74:D76)/SUM(E74:E76))</f>
         <v/>
       </c>
     </row>
@@ -2058,47 +2058,47 @@
         <v>17</v>
       </c>
       <c r="C85" s="6">
-        <f>SUM(C86:C107)/SUM(N86:N107)</f>
+        <f>IF(SUM(N86:N107)=0,0,(SUM(C86:C107)/SUM(N86:N107))</f>
         <v/>
       </c>
       <c r="D85" s="6">
-        <f>SUM(D86:D107)/SUM(N86:N107)</f>
+        <f>IF(SUM(N86:N107)=0,0,(SUM(D86:D107)/SUM(N86:N107))</f>
         <v/>
       </c>
       <c r="E85" s="6">
-        <f>SUM(E86:E107)/SUM(N86:N107)</f>
+        <f>IF(SUM(N86:N107)=0,0,(SUM(E86:E107)/SUM(N86:N107))</f>
         <v/>
       </c>
       <c r="F85" s="6">
-        <f>SUM(F86:F107)/SUM(N86:N107)</f>
+        <f>IF(SUM(N86:N107)=0,0,(SUM(F86:F107)/SUM(N86:N107))</f>
         <v/>
       </c>
       <c r="G85" s="6">
-        <f>SUM(G86:G107)/SUM(N86:N107)</f>
+        <f>IF(SUM(N86:N107)=0,0,(SUM(G86:G107)/SUM(N86:N107))</f>
         <v/>
       </c>
       <c r="H85" s="6">
-        <f>SUM(H86:H107)/SUM(N86:N107)</f>
+        <f>IF(SUM(N86:N107)=0,0,(SUM(H86:H107)/SUM(N86:N107))</f>
         <v/>
       </c>
       <c r="I85" s="6">
-        <f>SUM(I86:I107)/SUM(N86:N107)</f>
+        <f>IF(SUM(N86:N107)=0,0,(SUM(I86:I107)/SUM(N86:N107))</f>
         <v/>
       </c>
       <c r="J85" s="6">
-        <f>SUM(J86:J107)/SUM(N86:N107)</f>
+        <f>IF(SUM(N86:N107)=0,0,(SUM(J86:J107)/SUM(N86:N107))</f>
         <v/>
       </c>
       <c r="K85" s="6">
-        <f>SUM(K86:K107)/SUM(N86:N107)</f>
+        <f>IF(SUM(N86:N107)=0,0,(SUM(K86:K107)/SUM(N86:N107))</f>
         <v/>
       </c>
       <c r="L85" s="6">
-        <f>SUM(L86:L107)/SUM(N86:N107)</f>
+        <f>IF(SUM(N86:N107)=0,0,(SUM(L86:L107)/SUM(N86:N107))</f>
         <v/>
       </c>
       <c r="M85" s="6">
-        <f>SUM(M86:M107)/SUM(N86:N107)</f>
+        <f>IF(SUM(N86:N107)=0,0,(SUM(M86:M107)/SUM(N86:N107))</f>
         <v/>
       </c>
     </row>
@@ -3229,31 +3229,31 @@
         <v>17</v>
       </c>
       <c r="C110" s="6">
-        <f>SUM(C111:C132)/SUM(J111:J132)</f>
+        <f>IF(SUM(J111:J132)=0,0,(SUM(C111:C132)/SUM(J111:J132))</f>
         <v/>
       </c>
       <c r="D110" s="6">
-        <f>SUM(D111:D132)/SUM(J111:J132)</f>
+        <f>IF(SUM(J111:J132)=0,0,(SUM(D111:D132)/SUM(J111:J132))</f>
         <v/>
       </c>
       <c r="E110" s="6">
-        <f>SUM(E111:E132)/SUM(J111:J132)</f>
+        <f>IF(SUM(J111:J132)=0,0,(SUM(E111:E132)/SUM(J111:J132))</f>
         <v/>
       </c>
       <c r="F110" s="6">
-        <f>SUM(F111:F132)/SUM(J111:J132)</f>
+        <f>IF(SUM(J111:J132)=0,0,(SUM(F111:F132)/SUM(J111:J132))</f>
         <v/>
       </c>
       <c r="G110" s="6">
-        <f>SUM(G111:G132)/SUM(J111:J132)</f>
+        <f>IF(SUM(J111:J132)=0,0,(SUM(G111:G132)/SUM(J111:J132))</f>
         <v/>
       </c>
       <c r="H110" s="6">
-        <f>SUM(H111:H132)/SUM(J111:J132)</f>
+        <f>IF(SUM(J111:J132)=0,0,(SUM(H111:H132)/SUM(J111:J132))</f>
         <v/>
       </c>
       <c r="I110" s="6">
-        <f>SUM(I111:I132)/SUM(J111:J132)</f>
+        <f>IF(SUM(J111:J132)=0,0,(SUM(I111:I132)/SUM(J111:J132))</f>
         <v/>
       </c>
     </row>
@@ -4047,19 +4047,19 @@
         <v>17</v>
       </c>
       <c r="C135" s="6">
-        <f>SUM(C136:C157)/SUM(G136:G157)</f>
+        <f>IF(SUM(G136:G157)=0,0,(SUM(C136:C157)/SUM(G136:G157))</f>
         <v/>
       </c>
       <c r="D135" s="6">
-        <f>SUM(D136:D157)/SUM(G136:G157)</f>
+        <f>IF(SUM(G136:G157)=0,0,(SUM(D136:D157)/SUM(G136:G157))</f>
         <v/>
       </c>
       <c r="E135" s="6">
-        <f>SUM(E136:E157)/SUM(G136:G157)</f>
+        <f>IF(SUM(G136:G157)=0,0,(SUM(E136:E157)/SUM(G136:G157))</f>
         <v/>
       </c>
       <c r="F135" s="6">
-        <f>SUM(F136:F157)/SUM(G136:G157)</f>
+        <f>IF(SUM(G136:G157)=0,0,(SUM(F136:F157)/SUM(G136:G157))</f>
         <v/>
       </c>
     </row>
@@ -4662,35 +4662,35 @@
         <v>17</v>
       </c>
       <c r="C166" s="6">
-        <f>SUM(C167:C173)/SUM(K167:K173)</f>
+        <f>IF(SUM(K167:K173)=0,0,(SUM(C167:C173)/SUM(K167:K173))</f>
         <v/>
       </c>
       <c r="D166" s="6">
-        <f>SUM(D167:D173)/SUM(K167:K173)</f>
+        <f>IF(SUM(K167:K173)=0,0,(SUM(D167:D173)/SUM(K167:K173))</f>
         <v/>
       </c>
       <c r="E166" s="6">
-        <f>SUM(E167:E173)/SUM(K167:K173)</f>
+        <f>IF(SUM(K167:K173)=0,0,(SUM(E167:E173)/SUM(K167:K173))</f>
         <v/>
       </c>
       <c r="F166" s="6">
-        <f>SUM(F167:F173)/SUM(K167:K173)</f>
+        <f>IF(SUM(K167:K173)=0,0,(SUM(F167:F173)/SUM(K167:K173))</f>
         <v/>
       </c>
       <c r="G166" s="6">
-        <f>SUM(G167:G173)/SUM(K167:K173)</f>
+        <f>IF(SUM(K167:K173)=0,0,(SUM(G167:G173)/SUM(K167:K173))</f>
         <v/>
       </c>
       <c r="H166" s="6">
-        <f>SUM(H167:H173)/SUM(K167:K173)</f>
+        <f>IF(SUM(K167:K173)=0,0,(SUM(H167:H173)/SUM(K167:K173))</f>
         <v/>
       </c>
       <c r="I166" s="6">
-        <f>SUM(I167:I173)/SUM(K167:K173)</f>
+        <f>IF(SUM(K167:K173)=0,0,(SUM(I167:I173)/SUM(K167:K173))</f>
         <v/>
       </c>
       <c r="J166" s="6">
-        <f>SUM(J167:J173)/SUM(K167:K173)</f>
+        <f>IF(SUM(K167:K173)=0,0,(SUM(J167:J173)/SUM(K167:K173))</f>
         <v/>
       </c>
     </row>
@@ -5006,23 +5006,23 @@
         <v>17</v>
       </c>
       <c r="C176" s="6">
-        <f>SUM(C177:C183)/SUM(H177:H183)</f>
+        <f>IF(SUM(H177:H183)=0,0,(SUM(C177:C183)/SUM(H177:H183))</f>
         <v/>
       </c>
       <c r="D176" s="6">
-        <f>SUM(D177:D183)/SUM(H177:H183)</f>
+        <f>IF(SUM(H177:H183)=0,0,(SUM(D177:D183)/SUM(H177:H183))</f>
         <v/>
       </c>
       <c r="E176" s="6">
-        <f>SUM(E177:E183)/SUM(H177:H183)</f>
+        <f>IF(SUM(H177:H183)=0,0,(SUM(E177:E183)/SUM(H177:H183))</f>
         <v/>
       </c>
       <c r="F176" s="6">
-        <f>SUM(F177:F183)/SUM(H177:H183)</f>
+        <f>IF(SUM(H177:H183)=0,0,(SUM(F177:F183)/SUM(H177:H183))</f>
         <v/>
       </c>
       <c r="G176" s="6">
-        <f>SUM(G177:G183)/SUM(H177:H183)</f>
+        <f>IF(SUM(H177:H183)=0,0,(SUM(G177:G183)/SUM(H177:H183))</f>
         <v/>
       </c>
     </row>
@@ -5250,11 +5250,11 @@
         <v>17</v>
       </c>
       <c r="C186" s="6">
-        <f>SUM(C187:C193)/SUM(E187:E193)</f>
+        <f>IF(SUM(E187:E193)=0,0,(SUM(C187:C193)/SUM(E187:E193))</f>
         <v/>
       </c>
       <c r="D186" s="6">
-        <f>SUM(D187:D193)/SUM(E187:E193)</f>
+        <f>IF(SUM(E187:E193)=0,0,(SUM(D187:D193)/SUM(E187:E193))</f>
         <v/>
       </c>
     </row>
@@ -5427,19 +5427,19 @@
         <v>17</v>
       </c>
       <c r="C202" s="6">
-        <f>SUM(C203:C209)/SUM(G203:G209)</f>
+        <f>IF(SUM(G203:G209)=0,0,(SUM(C203:C209)/SUM(G203:G209))</f>
         <v/>
       </c>
       <c r="D202" s="6">
-        <f>SUM(D203:D209)/SUM(G203:G209)</f>
+        <f>IF(SUM(G203:G209)=0,0,(SUM(D203:D209)/SUM(G203:G209))</f>
         <v/>
       </c>
       <c r="E202" s="6">
-        <f>SUM(E203:E209)/SUM(G203:G209)</f>
+        <f>IF(SUM(G203:G209)=0,0,(SUM(E203:E209)/SUM(G203:G209))</f>
         <v/>
       </c>
       <c r="F202" s="6">
-        <f>SUM(F203:F209)/SUM(G203:G209)</f>
+        <f>IF(SUM(G203:G209)=0,0,(SUM(F203:F209)/SUM(G203:G209))</f>
         <v/>
       </c>
     </row>
@@ -5678,35 +5678,35 @@
         <v>17</v>
       </c>
       <c r="C212" s="6">
-        <f>SUM(C213:C219)/SUM(K213:K219)</f>
+        <f>IF(SUM(K213:K219)=0,0,(SUM(C213:C219)/SUM(K213:K219))</f>
         <v/>
       </c>
       <c r="D212" s="6">
-        <f>SUM(D213:D219)/SUM(K213:K219)</f>
+        <f>IF(SUM(K213:K219)=0,0,(SUM(D213:D219)/SUM(K213:K219))</f>
         <v/>
       </c>
       <c r="E212" s="6">
-        <f>SUM(E213:E219)/SUM(K213:K219)</f>
+        <f>IF(SUM(K213:K219)=0,0,(SUM(E213:E219)/SUM(K213:K219))</f>
         <v/>
       </c>
       <c r="F212" s="6">
-        <f>SUM(F213:F219)/SUM(K213:K219)</f>
+        <f>IF(SUM(K213:K219)=0,0,(SUM(F213:F219)/SUM(K213:K219))</f>
         <v/>
       </c>
       <c r="G212" s="6">
-        <f>SUM(G213:G219)/SUM(K213:K219)</f>
+        <f>IF(SUM(K213:K219)=0,0,(SUM(G213:G219)/SUM(K213:K219))</f>
         <v/>
       </c>
       <c r="H212" s="6">
-        <f>SUM(H213:H219)/SUM(K213:K219)</f>
+        <f>IF(SUM(K213:K219)=0,0,(SUM(H213:H219)/SUM(K213:K219))</f>
         <v/>
       </c>
       <c r="I212" s="6">
-        <f>SUM(I213:I219)/SUM(K213:K219)</f>
+        <f>IF(SUM(K213:K219)=0,0,(SUM(I213:I219)/SUM(K213:K219))</f>
         <v/>
       </c>
       <c r="J212" s="6">
-        <f>SUM(J213:J219)/SUM(K213:K219)</f>
+        <f>IF(SUM(K213:K219)=0,0,(SUM(J213:J219)/SUM(K213:K219))</f>
         <v/>
       </c>
     </row>
@@ -5999,15 +5999,15 @@
         <v>17</v>
       </c>
       <c r="C222" s="6">
-        <f>SUM(C223:C229)/SUM(F223:F229)</f>
+        <f>IF(SUM(F223:F229)=0,0,(SUM(C223:C229)/SUM(F223:F229))</f>
         <v/>
       </c>
       <c r="D222" s="6">
-        <f>SUM(D223:D229)/SUM(F223:F229)</f>
+        <f>IF(SUM(F223:F229)=0,0,(SUM(D223:D229)/SUM(F223:F229))</f>
         <v/>
       </c>
       <c r="E222" s="6">
-        <f>SUM(E223:E229)/SUM(F223:F229)</f>
+        <f>IF(SUM(F223:F229)=0,0,(SUM(E223:E229)/SUM(F223:F229))</f>
         <v/>
       </c>
     </row>
@@ -6217,43 +6217,43 @@
         <v>17</v>
       </c>
       <c r="C238" s="6">
-        <f>SUM(C239:C247)/SUM(M239:M247)</f>
+        <f>IF(SUM(M239:M247)=0,0,(SUM(C239:C247)/SUM(M239:M247))</f>
         <v/>
       </c>
       <c r="D238" s="6">
-        <f>SUM(D239:D247)/SUM(M239:M247)</f>
+        <f>IF(SUM(M239:M247)=0,0,(SUM(D239:D247)/SUM(M239:M247))</f>
         <v/>
       </c>
       <c r="E238" s="6">
-        <f>SUM(E239:E247)/SUM(M239:M247)</f>
+        <f>IF(SUM(M239:M247)=0,0,(SUM(E239:E247)/SUM(M239:M247))</f>
         <v/>
       </c>
       <c r="F238" s="6">
-        <f>SUM(F239:F247)/SUM(M239:M247)</f>
+        <f>IF(SUM(M239:M247)=0,0,(SUM(F239:F247)/SUM(M239:M247))</f>
         <v/>
       </c>
       <c r="G238" s="6">
-        <f>SUM(G239:G247)/SUM(M239:M247)</f>
+        <f>IF(SUM(M239:M247)=0,0,(SUM(G239:G247)/SUM(M239:M247))</f>
         <v/>
       </c>
       <c r="H238" s="6">
-        <f>SUM(H239:H247)/SUM(M239:M247)</f>
+        <f>IF(SUM(M239:M247)=0,0,(SUM(H239:H247)/SUM(M239:M247))</f>
         <v/>
       </c>
       <c r="I238" s="6">
-        <f>SUM(I239:I247)/SUM(M239:M247)</f>
+        <f>IF(SUM(M239:M247)=0,0,(SUM(I239:I247)/SUM(M239:M247))</f>
         <v/>
       </c>
       <c r="J238" s="6">
-        <f>SUM(J239:J247)/SUM(M239:M247)</f>
+        <f>IF(SUM(M239:M247)=0,0,(SUM(J239:J247)/SUM(M239:M247))</f>
         <v/>
       </c>
       <c r="K238" s="6">
-        <f>SUM(K239:K247)/SUM(M239:M247)</f>
+        <f>IF(SUM(M239:M247)=0,0,(SUM(K239:K247)/SUM(M239:M247))</f>
         <v/>
       </c>
       <c r="L238" s="6">
-        <f>SUM(L239:L247)/SUM(M239:M247)</f>
+        <f>IF(SUM(M239:M247)=0,0,(SUM(L239:L247)/SUM(M239:M247))</f>
         <v/>
       </c>
     </row>
@@ -6705,23 +6705,23 @@
         <v>17</v>
       </c>
       <c r="C250" s="6">
-        <f>SUM(C251:C259)/SUM(H251:H259)</f>
+        <f>IF(SUM(H251:H259)=0,0,(SUM(C251:C259)/SUM(H251:H259))</f>
         <v/>
       </c>
       <c r="D250" s="6">
-        <f>SUM(D251:D259)/SUM(H251:H259)</f>
+        <f>IF(SUM(H251:H259)=0,0,(SUM(D251:D259)/SUM(H251:H259))</f>
         <v/>
       </c>
       <c r="E250" s="6">
-        <f>SUM(E251:E259)/SUM(H251:H259)</f>
+        <f>IF(SUM(H251:H259)=0,0,(SUM(E251:E259)/SUM(H251:H259))</f>
         <v/>
       </c>
       <c r="F250" s="6">
-        <f>SUM(F251:F259)/SUM(H251:H259)</f>
+        <f>IF(SUM(H251:H259)=0,0,(SUM(F251:F259)/SUM(H251:H259))</f>
         <v/>
       </c>
       <c r="G250" s="6">
-        <f>SUM(G251:G259)/SUM(H251:H259)</f>
+        <f>IF(SUM(H251:H259)=0,0,(SUM(G251:G259)/SUM(H251:H259))</f>
         <v/>
       </c>
     </row>
@@ -7008,15 +7008,15 @@
         <v>17</v>
       </c>
       <c r="C262" s="6">
-        <f>SUM(C263:C271)/SUM(F263:F271)</f>
+        <f>IF(SUM(F263:F271)=0,0,(SUM(C263:C271)/SUM(F263:F271))</f>
         <v/>
       </c>
       <c r="D262" s="6">
-        <f>SUM(D263:D271)/SUM(F263:F271)</f>
+        <f>IF(SUM(F263:F271)=0,0,(SUM(D263:D271)/SUM(F263:F271))</f>
         <v/>
       </c>
       <c r="E262" s="6">
-        <f>SUM(E263:E271)/SUM(F263:F271)</f>
+        <f>IF(SUM(F263:F271)=0,0,(SUM(E263:E271)/SUM(F263:F271))</f>
         <v/>
       </c>
     </row>
@@ -7266,35 +7266,35 @@
         <v>17</v>
       </c>
       <c r="C280" s="6">
-        <f>SUM(C281:C284)/SUM(K281:K284)</f>
+        <f>IF(SUM(K281:K284)=0,0,(SUM(C281:C284)/SUM(K281:K284))</f>
         <v/>
       </c>
       <c r="D280" s="6">
-        <f>SUM(D281:D284)/SUM(K281:K284)</f>
+        <f>IF(SUM(K281:K284)=0,0,(SUM(D281:D284)/SUM(K281:K284))</f>
         <v/>
       </c>
       <c r="E280" s="6">
-        <f>SUM(E281:E284)/SUM(K281:K284)</f>
+        <f>IF(SUM(K281:K284)=0,0,(SUM(E281:E284)/SUM(K281:K284))</f>
         <v/>
       </c>
       <c r="F280" s="6">
-        <f>SUM(F281:F284)/SUM(K281:K284)</f>
+        <f>IF(SUM(K281:K284)=0,0,(SUM(F281:F284)/SUM(K281:K284))</f>
         <v/>
       </c>
       <c r="G280" s="6">
-        <f>SUM(G281:G284)/SUM(K281:K284)</f>
+        <f>IF(SUM(K281:K284)=0,0,(SUM(G281:G284)/SUM(K281:K284))</f>
         <v/>
       </c>
       <c r="H280" s="6">
-        <f>SUM(H281:H284)/SUM(K281:K284)</f>
+        <f>IF(SUM(K281:K284)=0,0,(SUM(H281:H284)/SUM(K281:K284))</f>
         <v/>
       </c>
       <c r="I280" s="6">
-        <f>SUM(I281:I284)/SUM(K281:K284)</f>
+        <f>IF(SUM(K281:K284)=0,0,(SUM(I281:I284)/SUM(K281:K284))</f>
         <v/>
       </c>
       <c r="J280" s="6">
-        <f>SUM(J281:J284)/SUM(K281:K284)</f>
+        <f>IF(SUM(K281:K284)=0,0,(SUM(J281:J284)/SUM(K281:K284))</f>
         <v/>
       </c>
     </row>
@@ -7488,19 +7488,19 @@
         <v>17</v>
       </c>
       <c r="C287" s="6">
-        <f>SUM(C288:C291)/SUM(G288:G291)</f>
+        <f>IF(SUM(G288:G291)=0,0,(SUM(C288:C291)/SUM(G288:G291))</f>
         <v/>
       </c>
       <c r="D287" s="6">
-        <f>SUM(D288:D291)/SUM(G288:G291)</f>
+        <f>IF(SUM(G288:G291)=0,0,(SUM(D288:D291)/SUM(G288:G291))</f>
         <v/>
       </c>
       <c r="E287" s="6">
-        <f>SUM(E288:E291)/SUM(G288:G291)</f>
+        <f>IF(SUM(G288:G291)=0,0,(SUM(E288:E291)/SUM(G288:G291))</f>
         <v/>
       </c>
       <c r="F287" s="6">
-        <f>SUM(F288:F291)/SUM(G288:G291)</f>
+        <f>IF(SUM(G288:G291)=0,0,(SUM(F288:F291)/SUM(G288:G291))</f>
         <v/>
       </c>
     </row>
@@ -7630,11 +7630,11 @@
         <v>17</v>
       </c>
       <c r="C294" s="6">
-        <f>SUM(C295:C298)/SUM(E295:E298)</f>
+        <f>IF(SUM(E295:E298)=0,0,(SUM(C295:C298)/SUM(E295:E298))</f>
         <v/>
       </c>
       <c r="D294" s="6">
-        <f>SUM(D295:D298)/SUM(E295:E298)</f>
+        <f>IF(SUM(E295:E298)=0,0,(SUM(D295:D298)/SUM(E295:E298))</f>
         <v/>
       </c>
     </row>
@@ -7761,35 +7761,35 @@
         <v>17</v>
       </c>
       <c r="C307" s="6">
-        <f>SUM(C308:C331)/SUM(K308:K331)</f>
+        <f>IF(SUM(K308:K331)=0,0,(SUM(C308:C331)/SUM(K308:K331))</f>
         <v/>
       </c>
       <c r="D307" s="6">
-        <f>SUM(D308:D331)/SUM(K308:K331)</f>
+        <f>IF(SUM(K308:K331)=0,0,(SUM(D308:D331)/SUM(K308:K331))</f>
         <v/>
       </c>
       <c r="E307" s="6">
-        <f>SUM(E308:E331)/SUM(K308:K331)</f>
+        <f>IF(SUM(K308:K331)=0,0,(SUM(E308:E331)/SUM(K308:K331))</f>
         <v/>
       </c>
       <c r="F307" s="6">
-        <f>SUM(F308:F331)/SUM(K308:K331)</f>
+        <f>IF(SUM(K308:K331)=0,0,(SUM(F308:F331)/SUM(K308:K331))</f>
         <v/>
       </c>
       <c r="G307" s="6">
-        <f>SUM(G308:G331)/SUM(K308:K331)</f>
+        <f>IF(SUM(K308:K331)=0,0,(SUM(G308:G331)/SUM(K308:K331))</f>
         <v/>
       </c>
       <c r="H307" s="6">
-        <f>SUM(H308:H331)/SUM(K308:K331)</f>
+        <f>IF(SUM(K308:K331)=0,0,(SUM(H308:H331)/SUM(K308:K331))</f>
         <v/>
       </c>
       <c r="I307" s="6">
-        <f>SUM(I308:I331)/SUM(K308:K331)</f>
+        <f>IF(SUM(K308:K331)=0,0,(SUM(I308:I331)/SUM(K308:K331))</f>
         <v/>
       </c>
       <c r="J307" s="6">
-        <f>SUM(J308:J331)/SUM(K308:K331)</f>
+        <f>IF(SUM(K308:K331)=0,0,(SUM(J308:J331)/SUM(K308:K331))</f>
         <v/>
       </c>
     </row>
@@ -8794,35 +8794,35 @@
         <v>17</v>
       </c>
       <c r="C334" s="6">
-        <f>SUM(C335:C358)/SUM(K335:K358)</f>
+        <f>IF(SUM(K335:K358)=0,0,(SUM(C335:C358)/SUM(K335:K358))</f>
         <v/>
       </c>
       <c r="D334" s="6">
-        <f>SUM(D335:D358)/SUM(K335:K358)</f>
+        <f>IF(SUM(K335:K358)=0,0,(SUM(D335:D358)/SUM(K335:K358))</f>
         <v/>
       </c>
       <c r="E334" s="6">
-        <f>SUM(E335:E358)/SUM(K335:K358)</f>
+        <f>IF(SUM(K335:K358)=0,0,(SUM(E335:E358)/SUM(K335:K358))</f>
         <v/>
       </c>
       <c r="F334" s="6">
-        <f>SUM(F335:F358)/SUM(K335:K358)</f>
+        <f>IF(SUM(K335:K358)=0,0,(SUM(F335:F358)/SUM(K335:K358))</f>
         <v/>
       </c>
       <c r="G334" s="6">
-        <f>SUM(G335:G358)/SUM(K335:K358)</f>
+        <f>IF(SUM(K335:K358)=0,0,(SUM(G335:G358)/SUM(K335:K358))</f>
         <v/>
       </c>
       <c r="H334" s="6">
-        <f>SUM(H335:H358)/SUM(K335:K358)</f>
+        <f>IF(SUM(K335:K358)=0,0,(SUM(H335:H358)/SUM(K335:K358))</f>
         <v/>
       </c>
       <c r="I334" s="6">
-        <f>SUM(I335:I358)/SUM(K335:K358)</f>
+        <f>IF(SUM(K335:K358)=0,0,(SUM(I335:I358)/SUM(K335:K358))</f>
         <v/>
       </c>
       <c r="J334" s="6">
-        <f>SUM(J335:J358)/SUM(K335:K358)</f>
+        <f>IF(SUM(K335:K358)=0,0,(SUM(J335:J358)/SUM(K335:K358))</f>
         <v/>
       </c>
     </row>
@@ -9760,15 +9760,15 @@
         <v>17</v>
       </c>
       <c r="C361" s="6">
-        <f>SUM(C362:C385)/SUM(F362:F385)</f>
+        <f>IF(SUM(F362:F385)=0,0,(SUM(C362:C385)/SUM(F362:F385))</f>
         <v/>
       </c>
       <c r="D361" s="6">
-        <f>SUM(D362:D385)/SUM(F362:F385)</f>
+        <f>IF(SUM(F362:F385)=0,0,(SUM(D362:D385)/SUM(F362:F385))</f>
         <v/>
       </c>
       <c r="E361" s="6">
-        <f>SUM(E362:E385)/SUM(F362:F385)</f>
+        <f>IF(SUM(F362:F385)=0,0,(SUM(E362:E385)/SUM(F362:F385))</f>
         <v/>
       </c>
     </row>
@@ -10357,47 +10357,47 @@
         <v>17</v>
       </c>
       <c r="C394" s="6">
-        <f>SUM(C395:C417)/SUM(N395:N417)</f>
+        <f>IF(SUM(N395:N417)=0,0,(SUM(C395:C417)/SUM(N395:N417))</f>
         <v/>
       </c>
       <c r="D394" s="6">
-        <f>SUM(D395:D417)/SUM(N395:N417)</f>
+        <f>IF(SUM(N395:N417)=0,0,(SUM(D395:D417)/SUM(N395:N417))</f>
         <v/>
       </c>
       <c r="E394" s="6">
-        <f>SUM(E395:E417)/SUM(N395:N417)</f>
+        <f>IF(SUM(N395:N417)=0,0,(SUM(E395:E417)/SUM(N395:N417))</f>
         <v/>
       </c>
       <c r="F394" s="6">
-        <f>SUM(F395:F417)/SUM(N395:N417)</f>
+        <f>IF(SUM(N395:N417)=0,0,(SUM(F395:F417)/SUM(N395:N417))</f>
         <v/>
       </c>
       <c r="G394" s="6">
-        <f>SUM(G395:G417)/SUM(N395:N417)</f>
+        <f>IF(SUM(N395:N417)=0,0,(SUM(G395:G417)/SUM(N395:N417))</f>
         <v/>
       </c>
       <c r="H394" s="6">
-        <f>SUM(H395:H417)/SUM(N395:N417)</f>
+        <f>IF(SUM(N395:N417)=0,0,(SUM(H395:H417)/SUM(N395:N417))</f>
         <v/>
       </c>
       <c r="I394" s="6">
-        <f>SUM(I395:I417)/SUM(N395:N417)</f>
+        <f>IF(SUM(N395:N417)=0,0,(SUM(I395:I417)/SUM(N395:N417))</f>
         <v/>
       </c>
       <c r="J394" s="6">
-        <f>SUM(J395:J417)/SUM(N395:N417)</f>
+        <f>IF(SUM(N395:N417)=0,0,(SUM(J395:J417)/SUM(N395:N417))</f>
         <v/>
       </c>
       <c r="K394" s="6">
-        <f>SUM(K395:K417)/SUM(N395:N417)</f>
+        <f>IF(SUM(N395:N417)=0,0,(SUM(K395:K417)/SUM(N395:N417))</f>
         <v/>
       </c>
       <c r="L394" s="6">
-        <f>SUM(L395:L417)/SUM(N395:N417)</f>
+        <f>IF(SUM(N395:N417)=0,0,(SUM(L395:L417)/SUM(N395:N417))</f>
         <v/>
       </c>
       <c r="M394" s="6">
-        <f>SUM(M395:M417)/SUM(N395:N417)</f>
+        <f>IF(SUM(N395:N417)=0,0,(SUM(M395:M417)/SUM(N395:N417))</f>
         <v/>
       </c>
     </row>
@@ -11579,31 +11579,31 @@
         <v>17</v>
       </c>
       <c r="C420" s="6">
-        <f>SUM(C421:C443)/SUM(J421:J443)</f>
+        <f>IF(SUM(J421:J443)=0,0,(SUM(C421:C443)/SUM(J421:J443))</f>
         <v/>
       </c>
       <c r="D420" s="6">
-        <f>SUM(D421:D443)/SUM(J421:J443)</f>
+        <f>IF(SUM(J421:J443)=0,0,(SUM(D421:D443)/SUM(J421:J443))</f>
         <v/>
       </c>
       <c r="E420" s="6">
-        <f>SUM(E421:E443)/SUM(J421:J443)</f>
+        <f>IF(SUM(J421:J443)=0,0,(SUM(E421:E443)/SUM(J421:J443))</f>
         <v/>
       </c>
       <c r="F420" s="6">
-        <f>SUM(F421:F443)/SUM(J421:J443)</f>
+        <f>IF(SUM(J421:J443)=0,0,(SUM(F421:F443)/SUM(J421:J443))</f>
         <v/>
       </c>
       <c r="G420" s="6">
-        <f>SUM(G421:G443)/SUM(J421:J443)</f>
+        <f>IF(SUM(J421:J443)=0,0,(SUM(G421:G443)/SUM(J421:J443))</f>
         <v/>
       </c>
       <c r="H420" s="6">
-        <f>SUM(H421:H443)/SUM(J421:J443)</f>
+        <f>IF(SUM(J421:J443)=0,0,(SUM(H421:H443)/SUM(J421:J443))</f>
         <v/>
       </c>
       <c r="I420" s="6">
-        <f>SUM(I421:I443)/SUM(J421:J443)</f>
+        <f>IF(SUM(J421:J443)=0,0,(SUM(I421:I443)/SUM(J421:J443))</f>
         <v/>
       </c>
     </row>
@@ -12432,19 +12432,19 @@
         <v>17</v>
       </c>
       <c r="C446" s="6">
-        <f>SUM(C447:C469)/SUM(G447:G469)</f>
+        <f>IF(SUM(G447:G469)=0,0,(SUM(C447:C469)/SUM(G447:G469))</f>
         <v/>
       </c>
       <c r="D446" s="6">
-        <f>SUM(D447:D469)/SUM(G447:G469)</f>
+        <f>IF(SUM(G447:G469)=0,0,(SUM(D447:D469)/SUM(G447:G469))</f>
         <v/>
       </c>
       <c r="E446" s="6">
-        <f>SUM(E447:E469)/SUM(G447:G469)</f>
+        <f>IF(SUM(G447:G469)=0,0,(SUM(E447:E469)/SUM(G447:G469))</f>
         <v/>
       </c>
       <c r="F446" s="6">
-        <f>SUM(F447:F469)/SUM(G447:G469)</f>
+        <f>IF(SUM(G447:G469)=0,0,(SUM(F447:F469)/SUM(G447:G469))</f>
         <v/>
       </c>
     </row>
@@ -13072,35 +13072,35 @@
         <v>17</v>
       </c>
       <c r="C478" s="6">
-        <f>SUM(C479:C482)/SUM(K479:K482)</f>
+        <f>IF(SUM(K479:K482)=0,0,(SUM(C479:C482)/SUM(K479:K482))</f>
         <v/>
       </c>
       <c r="D478" s="6">
-        <f>SUM(D479:D482)/SUM(K479:K482)</f>
+        <f>IF(SUM(K479:K482)=0,0,(SUM(D479:D482)/SUM(K479:K482))</f>
         <v/>
       </c>
       <c r="E478" s="6">
-        <f>SUM(E479:E482)/SUM(K479:K482)</f>
+        <f>IF(SUM(K479:K482)=0,0,(SUM(E479:E482)/SUM(K479:K482))</f>
         <v/>
       </c>
       <c r="F478" s="6">
-        <f>SUM(F479:F482)/SUM(K479:K482)</f>
+        <f>IF(SUM(K479:K482)=0,0,(SUM(F479:F482)/SUM(K479:K482))</f>
         <v/>
       </c>
       <c r="G478" s="6">
-        <f>SUM(G479:G482)/SUM(K479:K482)</f>
+        <f>IF(SUM(K479:K482)=0,0,(SUM(G479:G482)/SUM(K479:K482))</f>
         <v/>
       </c>
       <c r="H478" s="6">
-        <f>SUM(H479:H482)/SUM(K479:K482)</f>
+        <f>IF(SUM(K479:K482)=0,0,(SUM(H479:H482)/SUM(K479:K482))</f>
         <v/>
       </c>
       <c r="I478" s="6">
-        <f>SUM(I479:I482)/SUM(K479:K482)</f>
+        <f>IF(SUM(K479:K482)=0,0,(SUM(I479:I482)/SUM(K479:K482))</f>
         <v/>
       </c>
       <c r="J478" s="6">
-        <f>SUM(J479:J482)/SUM(K479:K482)</f>
+        <f>IF(SUM(K479:K482)=0,0,(SUM(J479:J482)/SUM(K479:K482))</f>
         <v/>
       </c>
     </row>
@@ -13292,19 +13292,19 @@
         <v>17</v>
       </c>
       <c r="C485" s="6">
-        <f>SUM(C486:C489)/SUM(G486:G489)</f>
+        <f>IF(SUM(G486:G489)=0,0,(SUM(C486:C489)/SUM(G486:G489))</f>
         <v/>
       </c>
       <c r="D485" s="6">
-        <f>SUM(D486:D489)/SUM(G486:G489)</f>
+        <f>IF(SUM(G486:G489)=0,0,(SUM(D486:D489)/SUM(G486:G489))</f>
         <v/>
       </c>
       <c r="E485" s="6">
-        <f>SUM(E486:E489)/SUM(G486:G489)</f>
+        <f>IF(SUM(G486:G489)=0,0,(SUM(E486:E489)/SUM(G486:G489))</f>
         <v/>
       </c>
       <c r="F485" s="6">
-        <f>SUM(F486:F489)/SUM(G486:G489)</f>
+        <f>IF(SUM(G486:G489)=0,0,(SUM(F486:F489)/SUM(G486:G489))</f>
         <v/>
       </c>
     </row>
@@ -13436,15 +13436,15 @@
         <v>17</v>
       </c>
       <c r="C492" s="6">
-        <f>SUM(C493:C496)/SUM(F493:F496)</f>
+        <f>IF(SUM(F493:F496)=0,0,(SUM(C493:C496)/SUM(F493:F496))</f>
         <v/>
       </c>
       <c r="D492" s="6">
-        <f>SUM(D493:D496)/SUM(F493:F496)</f>
+        <f>IF(SUM(F493:F496)=0,0,(SUM(D493:D496)/SUM(F493:F496))</f>
         <v/>
       </c>
       <c r="E492" s="6">
-        <f>SUM(E493:E496)/SUM(F493:F496)</f>
+        <f>IF(SUM(F493:F496)=0,0,(SUM(E493:E496)/SUM(F493:F496))</f>
         <v/>
       </c>
     </row>
@@ -13585,39 +13585,39 @@
         <v>17</v>
       </c>
       <c r="C505" s="6">
-        <f>SUM(C506:C513)/SUM(L506:L513)</f>
+        <f>IF(SUM(L506:L513)=0,0,(SUM(C506:C513)/SUM(L506:L513))</f>
         <v/>
       </c>
       <c r="D505" s="6">
-        <f>SUM(D506:D513)/SUM(L506:L513)</f>
+        <f>IF(SUM(L506:L513)=0,0,(SUM(D506:D513)/SUM(L506:L513))</f>
         <v/>
       </c>
       <c r="E505" s="6">
-        <f>SUM(E506:E513)/SUM(L506:L513)</f>
+        <f>IF(SUM(L506:L513)=0,0,(SUM(E506:E513)/SUM(L506:L513))</f>
         <v/>
       </c>
       <c r="F505" s="6">
-        <f>SUM(F506:F513)/SUM(L506:L513)</f>
+        <f>IF(SUM(L506:L513)=0,0,(SUM(F506:F513)/SUM(L506:L513))</f>
         <v/>
       </c>
       <c r="G505" s="6">
-        <f>SUM(G506:G513)/SUM(L506:L513)</f>
+        <f>IF(SUM(L506:L513)=0,0,(SUM(G506:G513)/SUM(L506:L513))</f>
         <v/>
       </c>
       <c r="H505" s="6">
-        <f>SUM(H506:H513)/SUM(L506:L513)</f>
+        <f>IF(SUM(L506:L513)=0,0,(SUM(H506:H513)/SUM(L506:L513))</f>
         <v/>
       </c>
       <c r="I505" s="6">
-        <f>SUM(I506:I513)/SUM(L506:L513)</f>
+        <f>IF(SUM(L506:L513)=0,0,(SUM(I506:I513)/SUM(L506:L513))</f>
         <v/>
       </c>
       <c r="J505" s="6">
-        <f>SUM(J506:J513)/SUM(L506:L513)</f>
+        <f>IF(SUM(L506:L513)=0,0,(SUM(J506:J513)/SUM(L506:L513))</f>
         <v/>
       </c>
       <c r="K505" s="6">
-        <f>SUM(K506:K513)/SUM(L506:L513)</f>
+        <f>IF(SUM(L506:L513)=0,0,(SUM(K506:K513)/SUM(L506:L513))</f>
         <v/>
       </c>
     </row>
@@ -13992,19 +13992,19 @@
         <v>17</v>
       </c>
       <c r="C516" s="6">
-        <f>SUM(C517:C524)/SUM(G517:G524)</f>
+        <f>IF(SUM(G517:G524)=0,0,(SUM(C517:C524)/SUM(G517:G524))</f>
         <v/>
       </c>
       <c r="D516" s="6">
-        <f>SUM(D517:D524)/SUM(G517:G524)</f>
+        <f>IF(SUM(G517:G524)=0,0,(SUM(D517:D524)/SUM(G517:G524))</f>
         <v/>
       </c>
       <c r="E516" s="6">
-        <f>SUM(E517:E524)/SUM(G517:G524)</f>
+        <f>IF(SUM(G517:G524)=0,0,(SUM(E517:E524)/SUM(G517:G524))</f>
         <v/>
       </c>
       <c r="F516" s="6">
-        <f>SUM(F517:F524)/SUM(G517:G524)</f>
+        <f>IF(SUM(G517:G524)=0,0,(SUM(F517:F524)/SUM(G517:G524))</f>
         <v/>
       </c>
     </row>
@@ -14233,11 +14233,11 @@
         <v>17</v>
       </c>
       <c r="C527" s="6">
-        <f>SUM(C528:C535)/SUM(E528:E535)</f>
+        <f>IF(SUM(E528:E535)=0,0,(SUM(C528:C535)/SUM(E528:E535))</f>
         <v/>
       </c>
       <c r="D527" s="6">
-        <f>SUM(D528:D535)/SUM(E528:E535)</f>
+        <f>IF(SUM(E528:E535)=0,0,(SUM(D528:D535)/SUM(E528:E535))</f>
         <v/>
       </c>
     </row>
@@ -14444,39 +14444,39 @@
         <v>17</v>
       </c>
       <c r="C544" s="6">
-        <f>SUM(C545:C550)/SUM(L545:L550)</f>
+        <f>IF(SUM(L545:L550)=0,0,(SUM(C545:C550)/SUM(L545:L550))</f>
         <v/>
       </c>
       <c r="D544" s="6">
-        <f>SUM(D545:D550)/SUM(L545:L550)</f>
+        <f>IF(SUM(L545:L550)=0,0,(SUM(D545:D550)/SUM(L545:L550))</f>
         <v/>
       </c>
       <c r="E544" s="6">
-        <f>SUM(E545:E550)/SUM(L545:L550)</f>
+        <f>IF(SUM(L545:L550)=0,0,(SUM(E545:E550)/SUM(L545:L550))</f>
         <v/>
       </c>
       <c r="F544" s="6">
-        <f>SUM(F545:F550)/SUM(L545:L550)</f>
+        <f>IF(SUM(L545:L550)=0,0,(SUM(F545:F550)/SUM(L545:L550))</f>
         <v/>
       </c>
       <c r="G544" s="6">
-        <f>SUM(G545:G550)/SUM(L545:L550)</f>
+        <f>IF(SUM(L545:L550)=0,0,(SUM(G545:G550)/SUM(L545:L550))</f>
         <v/>
       </c>
       <c r="H544" s="6">
-        <f>SUM(H545:H550)/SUM(L545:L550)</f>
+        <f>IF(SUM(L545:L550)=0,0,(SUM(H545:H550)/SUM(L545:L550))</f>
         <v/>
       </c>
       <c r="I544" s="6">
-        <f>SUM(I545:I550)/SUM(L545:L550)</f>
+        <f>IF(SUM(L545:L550)=0,0,(SUM(I545:I550)/SUM(L545:L550))</f>
         <v/>
       </c>
       <c r="J544" s="6">
-        <f>SUM(J545:J550)/SUM(L545:L550)</f>
+        <f>IF(SUM(L545:L550)=0,0,(SUM(J545:J550)/SUM(L545:L550))</f>
         <v/>
       </c>
       <c r="K544" s="6">
-        <f>SUM(K545:K550)/SUM(L545:L550)</f>
+        <f>IF(SUM(L545:L550)=0,0,(SUM(K545:K550)/SUM(L545:L550))</f>
         <v/>
       </c>
     </row>
@@ -14776,27 +14776,27 @@
         <v>17</v>
       </c>
       <c r="C553" s="6">
-        <f>SUM(C554:C559)/SUM(I554:I559)</f>
+        <f>IF(SUM(I554:I559)=0,0,(SUM(C554:C559)/SUM(I554:I559))</f>
         <v/>
       </c>
       <c r="D553" s="6">
-        <f>SUM(D554:D559)/SUM(I554:I559)</f>
+        <f>IF(SUM(I554:I559)=0,0,(SUM(D554:D559)/SUM(I554:I559))</f>
         <v/>
       </c>
       <c r="E553" s="6">
-        <f>SUM(E554:E559)/SUM(I554:I559)</f>
+        <f>IF(SUM(I554:I559)=0,0,(SUM(E554:E559)/SUM(I554:I559))</f>
         <v/>
       </c>
       <c r="F553" s="6">
-        <f>SUM(F554:F559)/SUM(I554:I559)</f>
+        <f>IF(SUM(I554:I559)=0,0,(SUM(F554:F559)/SUM(I554:I559))</f>
         <v/>
       </c>
       <c r="G553" s="6">
-        <f>SUM(G554:G559)/SUM(I554:I559)</f>
+        <f>IF(SUM(I554:I559)=0,0,(SUM(G554:G559)/SUM(I554:I559))</f>
         <v/>
       </c>
       <c r="H553" s="6">
-        <f>SUM(H554:H559)/SUM(I554:I559)</f>
+        <f>IF(SUM(I554:I559)=0,0,(SUM(H554:H559)/SUM(I554:I559))</f>
         <v/>
       </c>
     </row>
@@ -15015,15 +15015,15 @@
         <v>17</v>
       </c>
       <c r="C562" s="6">
-        <f>SUM(C563:C568)/SUM(F563:F568)</f>
+        <f>IF(SUM(F563:F568)=0,0,(SUM(C563:C568)/SUM(F563:F568))</f>
         <v/>
       </c>
       <c r="D562" s="6">
-        <f>SUM(D563:D568)/SUM(F563:F568)</f>
+        <f>IF(SUM(F563:F568)=0,0,(SUM(D563:D568)/SUM(F563:F568))</f>
         <v/>
       </c>
       <c r="E562" s="6">
-        <f>SUM(E563:E568)/SUM(F563:F568)</f>
+        <f>IF(SUM(F563:F568)=0,0,(SUM(E563:E568)/SUM(F563:F568))</f>
         <v/>
       </c>
     </row>
@@ -15194,19 +15194,19 @@
         <v>17</v>
       </c>
       <c r="C577" s="6">
-        <f>SUM(C578:C581)/SUM(G578:G581)</f>
+        <f>IF(SUM(G578:G581)=0,0,(SUM(C578:C581)/SUM(G578:G581))</f>
         <v/>
       </c>
       <c r="D577" s="6">
-        <f>SUM(D578:D581)/SUM(G578:G581)</f>
+        <f>IF(SUM(G578:G581)=0,0,(SUM(D578:D581)/SUM(G578:G581))</f>
         <v/>
       </c>
       <c r="E577" s="6">
-        <f>SUM(E578:E581)/SUM(G578:G581)</f>
+        <f>IF(SUM(G578:G581)=0,0,(SUM(E578:E581)/SUM(G578:G581))</f>
         <v/>
       </c>
       <c r="F577" s="6">
-        <f>SUM(F578:F581)/SUM(G578:G581)</f>
+        <f>IF(SUM(G578:G581)=0,0,(SUM(F578:F581)/SUM(G578:G581))</f>
         <v/>
       </c>
     </row>
@@ -15344,11 +15344,11 @@
         <v>17</v>
       </c>
       <c r="C584" s="6">
-        <f>SUM(C585:C588)/SUM(E585:E588)</f>
+        <f>IF(SUM(E585:E588)=0,0,(SUM(C585:C588)/SUM(E585:E588))</f>
         <v/>
       </c>
       <c r="D584" s="6">
-        <f>SUM(D585:D588)/SUM(E585:E588)</f>
+        <f>IF(SUM(E585:E588)=0,0,(SUM(D585:D588)/SUM(E585:E588))</f>
         <v/>
       </c>
     </row>
@@ -15452,11 +15452,11 @@
         <v>17</v>
       </c>
       <c r="C591" s="6">
-        <f>SUM(C592:C595)/SUM(E592:E595)</f>
+        <f>IF(SUM(E592:E595)=0,0,(SUM(C592:C595)/SUM(E592:E595))</f>
         <v/>
       </c>
       <c r="D591" s="6">
-        <f>SUM(D592:D595)/SUM(E592:E595)</f>
+        <f>IF(SUM(E592:E595)=0,0,(SUM(D592:D595)/SUM(E592:E595))</f>
         <v/>
       </c>
     </row>
@@ -15588,39 +15588,39 @@
         <v>17</v>
       </c>
       <c r="C604" s="6">
-        <f>SUM(C605:C631)/SUM(L605:L631)</f>
+        <f>IF(SUM(L605:L631)=0,0,(SUM(C605:C631)/SUM(L605:L631))</f>
         <v/>
       </c>
       <c r="D604" s="6">
-        <f>SUM(D605:D631)/SUM(L605:L631)</f>
+        <f>IF(SUM(L605:L631)=0,0,(SUM(D605:D631)/SUM(L605:L631))</f>
         <v/>
       </c>
       <c r="E604" s="6">
-        <f>SUM(E605:E631)/SUM(L605:L631)</f>
+        <f>IF(SUM(L605:L631)=0,0,(SUM(E605:E631)/SUM(L605:L631))</f>
         <v/>
       </c>
       <c r="F604" s="6">
-        <f>SUM(F605:F631)/SUM(L605:L631)</f>
+        <f>IF(SUM(L605:L631)=0,0,(SUM(F605:F631)/SUM(L605:L631))</f>
         <v/>
       </c>
       <c r="G604" s="6">
-        <f>SUM(G605:G631)/SUM(L605:L631)</f>
+        <f>IF(SUM(L605:L631)=0,0,(SUM(G605:G631)/SUM(L605:L631))</f>
         <v/>
       </c>
       <c r="H604" s="6">
-        <f>SUM(H605:H631)/SUM(L605:L631)</f>
+        <f>IF(SUM(L605:L631)=0,0,(SUM(H605:H631)/SUM(L605:L631))</f>
         <v/>
       </c>
       <c r="I604" s="6">
-        <f>SUM(I605:I631)/SUM(L605:L631)</f>
+        <f>IF(SUM(L605:L631)=0,0,(SUM(I605:I631)/SUM(L605:L631))</f>
         <v/>
       </c>
       <c r="J604" s="6">
-        <f>SUM(J605:J631)/SUM(L605:L631)</f>
+        <f>IF(SUM(L605:L631)=0,0,(SUM(J605:J631)/SUM(L605:L631))</f>
         <v/>
       </c>
       <c r="K604" s="6">
-        <f>SUM(K605:K631)/SUM(L605:L631)</f>
+        <f>IF(SUM(L605:L631)=0,0,(SUM(K605:K631)/SUM(L605:L631))</f>
         <v/>
       </c>
     </row>
@@ -16837,47 +16837,47 @@
         <v>17</v>
       </c>
       <c r="C634" s="6">
-        <f>SUM(C635:C661)/SUM(N635:N661)</f>
+        <f>IF(SUM(N635:N661)=0,0,(SUM(C635:C661)/SUM(N635:N661))</f>
         <v/>
       </c>
       <c r="D634" s="6">
-        <f>SUM(D635:D661)/SUM(N635:N661)</f>
+        <f>IF(SUM(N635:N661)=0,0,(SUM(D635:D661)/SUM(N635:N661))</f>
         <v/>
       </c>
       <c r="E634" s="6">
-        <f>SUM(E635:E661)/SUM(N635:N661)</f>
+        <f>IF(SUM(N635:N661)=0,0,(SUM(E635:E661)/SUM(N635:N661))</f>
         <v/>
       </c>
       <c r="F634" s="6">
-        <f>SUM(F635:F661)/SUM(N635:N661)</f>
+        <f>IF(SUM(N635:N661)=0,0,(SUM(F635:F661)/SUM(N635:N661))</f>
         <v/>
       </c>
       <c r="G634" s="6">
-        <f>SUM(G635:G661)/SUM(N635:N661)</f>
+        <f>IF(SUM(N635:N661)=0,0,(SUM(G635:G661)/SUM(N635:N661))</f>
         <v/>
       </c>
       <c r="H634" s="6">
-        <f>SUM(H635:H661)/SUM(N635:N661)</f>
+        <f>IF(SUM(N635:N661)=0,0,(SUM(H635:H661)/SUM(N635:N661))</f>
         <v/>
       </c>
       <c r="I634" s="6">
-        <f>SUM(I635:I661)/SUM(N635:N661)</f>
+        <f>IF(SUM(N635:N661)=0,0,(SUM(I635:I661)/SUM(N635:N661))</f>
         <v/>
       </c>
       <c r="J634" s="6">
-        <f>SUM(J635:J661)/SUM(N635:N661)</f>
+        <f>IF(SUM(N635:N661)=0,0,(SUM(J635:J661)/SUM(N635:N661))</f>
         <v/>
       </c>
       <c r="K634" s="6">
-        <f>SUM(K635:K661)/SUM(N635:N661)</f>
+        <f>IF(SUM(N635:N661)=0,0,(SUM(K635:K661)/SUM(N635:N661))</f>
         <v/>
       </c>
       <c r="L634" s="6">
-        <f>SUM(L635:L661)/SUM(N635:N661)</f>
+        <f>IF(SUM(N635:N661)=0,0,(SUM(L635:L661)/SUM(N635:N661))</f>
         <v/>
       </c>
       <c r="M634" s="6">
-        <f>SUM(M635:M661)/SUM(N635:N661)</f>
+        <f>IF(SUM(N635:N661)=0,0,(SUM(M635:M661)/SUM(N635:N661))</f>
         <v/>
       </c>
     </row>
@@ -18181,27 +18181,27 @@
         <v>17</v>
       </c>
       <c r="C664" s="6">
-        <f>SUM(C665:C691)/SUM(I665:I691)</f>
+        <f>IF(SUM(I665:I691)=0,0,(SUM(C665:C691)/SUM(I665:I691))</f>
         <v/>
       </c>
       <c r="D664" s="6">
-        <f>SUM(D665:D691)/SUM(I665:I691)</f>
+        <f>IF(SUM(I665:I691)=0,0,(SUM(D665:D691)/SUM(I665:I691))</f>
         <v/>
       </c>
       <c r="E664" s="6">
-        <f>SUM(E665:E691)/SUM(I665:I691)</f>
+        <f>IF(SUM(I665:I691)=0,0,(SUM(E665:E691)/SUM(I665:I691))</f>
         <v/>
       </c>
       <c r="F664" s="6">
-        <f>SUM(F665:F691)/SUM(I665:I691)</f>
+        <f>IF(SUM(I665:I691)=0,0,(SUM(F665:F691)/SUM(I665:I691))</f>
         <v/>
       </c>
       <c r="G664" s="6">
-        <f>SUM(G665:G691)/SUM(I665:I691)</f>
+        <f>IF(SUM(I665:I691)=0,0,(SUM(G665:G691)/SUM(I665:I691))</f>
         <v/>
       </c>
       <c r="H664" s="6">
-        <f>SUM(H665:H691)/SUM(I665:I691)</f>
+        <f>IF(SUM(I665:I691)=0,0,(SUM(H665:H691)/SUM(I665:I691))</f>
         <v/>
       </c>
     </row>
@@ -19081,23 +19081,23 @@
         <v>17</v>
       </c>
       <c r="C700" s="6">
-        <f>SUM(C701:C703)/SUM(H701:H703)</f>
+        <f>IF(SUM(H701:H703)=0,0,(SUM(C701:C703)/SUM(H701:H703))</f>
         <v/>
       </c>
       <c r="D700" s="6">
-        <f>SUM(D701:D703)/SUM(H701:H703)</f>
+        <f>IF(SUM(H701:H703)=0,0,(SUM(D701:D703)/SUM(H701:H703))</f>
         <v/>
       </c>
       <c r="E700" s="6">
-        <f>SUM(E701:E703)/SUM(H701:H703)</f>
+        <f>IF(SUM(H701:H703)=0,0,(SUM(E701:E703)/SUM(H701:H703))</f>
         <v/>
       </c>
       <c r="F700" s="6">
-        <f>SUM(F701:F703)/SUM(H701:H703)</f>
+        <f>IF(SUM(H701:H703)=0,0,(SUM(F701:F703)/SUM(H701:H703))</f>
         <v/>
       </c>
       <c r="G700" s="6">
-        <f>SUM(G701:G703)/SUM(H701:H703)</f>
+        <f>IF(SUM(H701:H703)=0,0,(SUM(G701:G703)/SUM(H701:H703))</f>
         <v/>
       </c>
     </row>
@@ -19216,15 +19216,15 @@
         <v>17</v>
       </c>
       <c r="C706" s="6">
-        <f>SUM(C707:C709)/SUM(F707:F709)</f>
+        <f>IF(SUM(F707:F709)=0,0,(SUM(C707:C709)/SUM(F707:F709))</f>
         <v/>
       </c>
       <c r="D706" s="6">
-        <f>SUM(D707:D709)/SUM(F707:F709)</f>
+        <f>IF(SUM(F707:F709)=0,0,(SUM(D707:D709)/SUM(F707:F709))</f>
         <v/>
       </c>
       <c r="E706" s="6">
-        <f>SUM(E707:E709)/SUM(F707:F709)</f>
+        <f>IF(SUM(F707:F709)=0,0,(SUM(E707:E709)/SUM(F707:F709))</f>
         <v/>
       </c>
     </row>
@@ -19316,11 +19316,11 @@
         <v>17</v>
       </c>
       <c r="C712" s="6">
-        <f>SUM(C713:C715)/SUM(E713:E715)</f>
+        <f>IF(SUM(E713:E715)=0,0,(SUM(C713:C715)/SUM(E713:E715))</f>
         <v/>
       </c>
       <c r="D712" s="6">
-        <f>SUM(D713:D715)/SUM(E713:E715)</f>
+        <f>IF(SUM(E713:E715)=0,0,(SUM(D713:D715)/SUM(E713:E715))</f>
         <v/>
       </c>
     </row>
@@ -19415,19 +19415,19 @@
         <v>17</v>
       </c>
       <c r="C724" s="6">
-        <f>SUM(C725:C733)/SUM(G725:G733)</f>
+        <f>IF(SUM(G725:G733)=0,0,(SUM(C725:C733)/SUM(G725:G733))</f>
         <v/>
       </c>
       <c r="D724" s="6">
-        <f>SUM(D725:D733)/SUM(G725:G733)</f>
+        <f>IF(SUM(G725:G733)=0,0,(SUM(D725:D733)/SUM(G725:G733))</f>
         <v/>
       </c>
       <c r="E724" s="6">
-        <f>SUM(E725:E733)/SUM(G725:G733)</f>
+        <f>IF(SUM(G725:G733)=0,0,(SUM(E725:E733)/SUM(G725:G733))</f>
         <v/>
       </c>
       <c r="F724" s="6">
-        <f>SUM(F725:F733)/SUM(G725:G733)</f>
+        <f>IF(SUM(G725:G733)=0,0,(SUM(F725:F733)/SUM(G725:G733))</f>
         <v/>
       </c>
     </row>
@@ -19723,35 +19723,35 @@
         <v>17</v>
       </c>
       <c r="C736" s="6">
-        <f>SUM(C737:C745)/SUM(K737:K745)</f>
+        <f>IF(SUM(K737:K745)=0,0,(SUM(C737:C745)/SUM(K737:K745))</f>
         <v/>
       </c>
       <c r="D736" s="6">
-        <f>SUM(D737:D745)/SUM(K737:K745)</f>
+        <f>IF(SUM(K737:K745)=0,0,(SUM(D737:D745)/SUM(K737:K745))</f>
         <v/>
       </c>
       <c r="E736" s="6">
-        <f>SUM(E737:E745)/SUM(K737:K745)</f>
+        <f>IF(SUM(K737:K745)=0,0,(SUM(E737:E745)/SUM(K737:K745))</f>
         <v/>
       </c>
       <c r="F736" s="6">
-        <f>SUM(F737:F745)/SUM(K737:K745)</f>
+        <f>IF(SUM(K737:K745)=0,0,(SUM(F737:F745)/SUM(K737:K745))</f>
         <v/>
       </c>
       <c r="G736" s="6">
-        <f>SUM(G737:G745)/SUM(K737:K745)</f>
+        <f>IF(SUM(K737:K745)=0,0,(SUM(G737:G745)/SUM(K737:K745))</f>
         <v/>
       </c>
       <c r="H736" s="6">
-        <f>SUM(H737:H745)/SUM(K737:K745)</f>
+        <f>IF(SUM(K737:K745)=0,0,(SUM(H737:H745)/SUM(K737:K745))</f>
         <v/>
       </c>
       <c r="I736" s="6">
-        <f>SUM(I737:I745)/SUM(K737:K745)</f>
+        <f>IF(SUM(K737:K745)=0,0,(SUM(I737:I745)/SUM(K737:K745))</f>
         <v/>
       </c>
       <c r="J736" s="6">
-        <f>SUM(J737:J745)/SUM(K737:K745)</f>
+        <f>IF(SUM(K737:K745)=0,0,(SUM(J737:J745)/SUM(K737:K745))</f>
         <v/>
       </c>
     </row>
@@ -20117,11 +20117,11 @@
         <v>17</v>
       </c>
       <c r="C748" s="6">
-        <f>SUM(C749:C757)/SUM(E749:E757)</f>
+        <f>IF(SUM(E749:E757)=0,0,(SUM(C749:C757)/SUM(E749:E757))</f>
         <v/>
       </c>
       <c r="D748" s="6">
-        <f>SUM(D749:D757)/SUM(E749:E757)</f>
+        <f>IF(SUM(E749:E757)=0,0,(SUM(D749:D757)/SUM(E749:E757))</f>
         <v/>
       </c>
     </row>
@@ -20338,31 +20338,31 @@
         <v>17</v>
       </c>
       <c r="C766" s="6">
-        <f>SUM(C767:C770)/SUM(J767:J770)</f>
+        <f>IF(SUM(J767:J770)=0,0,(SUM(C767:C770)/SUM(J767:J770))</f>
         <v/>
       </c>
       <c r="D766" s="6">
-        <f>SUM(D767:D770)/SUM(J767:J770)</f>
+        <f>IF(SUM(J767:J770)=0,0,(SUM(D767:D770)/SUM(J767:J770))</f>
         <v/>
       </c>
       <c r="E766" s="6">
-        <f>SUM(E767:E770)/SUM(J767:J770)</f>
+        <f>IF(SUM(J767:J770)=0,0,(SUM(E767:E770)/SUM(J767:J770))</f>
         <v/>
       </c>
       <c r="F766" s="6">
-        <f>SUM(F767:F770)/SUM(J767:J770)</f>
+        <f>IF(SUM(J767:J770)=0,0,(SUM(F767:F770)/SUM(J767:J770))</f>
         <v/>
       </c>
       <c r="G766" s="6">
-        <f>SUM(G767:G770)/SUM(J767:J770)</f>
+        <f>IF(SUM(J767:J770)=0,0,(SUM(G767:G770)/SUM(J767:J770))</f>
         <v/>
       </c>
       <c r="H766" s="6">
-        <f>SUM(H767:H770)/SUM(J767:J770)</f>
+        <f>IF(SUM(J767:J770)=0,0,(SUM(H767:H770)/SUM(J767:J770))</f>
         <v/>
       </c>
       <c r="I766" s="6">
-        <f>SUM(I767:I770)/SUM(J767:J770)</f>
+        <f>IF(SUM(J767:J770)=0,0,(SUM(I767:I770)/SUM(J767:J770))</f>
         <v/>
       </c>
     </row>
@@ -20542,15 +20542,15 @@
         <v>17</v>
       </c>
       <c r="C773" s="6">
-        <f>SUM(C774:C777)/SUM(F774:F777)</f>
+        <f>IF(SUM(F774:F777)=0,0,(SUM(C774:C777)/SUM(F774:F777))</f>
         <v/>
       </c>
       <c r="D773" s="6">
-        <f>SUM(D774:D777)/SUM(F774:F777)</f>
+        <f>IF(SUM(F774:F777)=0,0,(SUM(D774:D777)/SUM(F774:F777))</f>
         <v/>
       </c>
       <c r="E773" s="6">
-        <f>SUM(E774:E777)/SUM(F774:F777)</f>
+        <f>IF(SUM(F774:F777)=0,0,(SUM(E774:E777)/SUM(F774:F777))</f>
         <v/>
       </c>
     </row>
@@ -20666,11 +20666,11 @@
         <v>17</v>
       </c>
       <c r="C780" s="6">
-        <f>SUM(C781:C784)/SUM(E781:E784)</f>
+        <f>IF(SUM(E781:E784)=0,0,(SUM(C781:C784)/SUM(E781:E784))</f>
         <v/>
       </c>
       <c r="D780" s="6">
-        <f>SUM(D781:D784)/SUM(E781:E784)</f>
+        <f>IF(SUM(E781:E784)=0,0,(SUM(D781:D784)/SUM(E781:E784))</f>
         <v/>
       </c>
     </row>
@@ -20806,47 +20806,47 @@
         <v>17</v>
       </c>
       <c r="C793" s="6">
-        <f>SUM(C794:C805)/SUM(N794:N805)</f>
+        <f>IF(SUM(N794:N805)=0,0,(SUM(C794:C805)/SUM(N794:N805))</f>
         <v/>
       </c>
       <c r="D793" s="6">
-        <f>SUM(D794:D805)/SUM(N794:N805)</f>
+        <f>IF(SUM(N794:N805)=0,0,(SUM(D794:D805)/SUM(N794:N805))</f>
         <v/>
       </c>
       <c r="E793" s="6">
-        <f>SUM(E794:E805)/SUM(N794:N805)</f>
+        <f>IF(SUM(N794:N805)=0,0,(SUM(E794:E805)/SUM(N794:N805))</f>
         <v/>
       </c>
       <c r="F793" s="6">
-        <f>SUM(F794:F805)/SUM(N794:N805)</f>
+        <f>IF(SUM(N794:N805)=0,0,(SUM(F794:F805)/SUM(N794:N805))</f>
         <v/>
       </c>
       <c r="G793" s="6">
-        <f>SUM(G794:G805)/SUM(N794:N805)</f>
+        <f>IF(SUM(N794:N805)=0,0,(SUM(G794:G805)/SUM(N794:N805))</f>
         <v/>
       </c>
       <c r="H793" s="6">
-        <f>SUM(H794:H805)/SUM(N794:N805)</f>
+        <f>IF(SUM(N794:N805)=0,0,(SUM(H794:H805)/SUM(N794:N805))</f>
         <v/>
       </c>
       <c r="I793" s="6">
-        <f>SUM(I794:I805)/SUM(N794:N805)</f>
+        <f>IF(SUM(N794:N805)=0,0,(SUM(I794:I805)/SUM(N794:N805))</f>
         <v/>
       </c>
       <c r="J793" s="6">
-        <f>SUM(J794:J805)/SUM(N794:N805)</f>
+        <f>IF(SUM(N794:N805)=0,0,(SUM(J794:J805)/SUM(N794:N805))</f>
         <v/>
       </c>
       <c r="K793" s="6">
-        <f>SUM(K794:K805)/SUM(N794:N805)</f>
+        <f>IF(SUM(N794:N805)=0,0,(SUM(K794:K805)/SUM(N794:N805))</f>
         <v/>
       </c>
       <c r="L793" s="6">
-        <f>SUM(L794:L805)/SUM(N794:N805)</f>
+        <f>IF(SUM(N794:N805)=0,0,(SUM(L794:L805)/SUM(N794:N805))</f>
         <v/>
       </c>
       <c r="M793" s="6">
-        <f>SUM(M794:M805)/SUM(N794:N805)</f>
+        <f>IF(SUM(N794:N805)=0,0,(SUM(M794:M805)/SUM(N794:N805))</f>
         <v/>
       </c>
     </row>
@@ -21475,27 +21475,27 @@
         <v>17</v>
       </c>
       <c r="C808" s="6">
-        <f>SUM(C809:C820)/SUM(I809:I820)</f>
+        <f>IF(SUM(I809:I820)=0,0,(SUM(C809:C820)/SUM(I809:I820))</f>
         <v/>
       </c>
       <c r="D808" s="6">
-        <f>SUM(D809:D820)/SUM(I809:I820)</f>
+        <f>IF(SUM(I809:I820)=0,0,(SUM(D809:D820)/SUM(I809:I820))</f>
         <v/>
       </c>
       <c r="E808" s="6">
-        <f>SUM(E809:E820)/SUM(I809:I820)</f>
+        <f>IF(SUM(I809:I820)=0,0,(SUM(E809:E820)/SUM(I809:I820))</f>
         <v/>
       </c>
       <c r="F808" s="6">
-        <f>SUM(F809:F820)/SUM(I809:I820)</f>
+        <f>IF(SUM(I809:I820)=0,0,(SUM(F809:F820)/SUM(I809:I820))</f>
         <v/>
       </c>
       <c r="G808" s="6">
-        <f>SUM(G809:G820)/SUM(I809:I820)</f>
+        <f>IF(SUM(I809:I820)=0,0,(SUM(G809:G820)/SUM(I809:I820))</f>
         <v/>
       </c>
       <c r="H808" s="6">
-        <f>SUM(H809:H820)/SUM(I809:I820)</f>
+        <f>IF(SUM(I809:I820)=0,0,(SUM(H809:H820)/SUM(I809:I820))</f>
         <v/>
       </c>
     </row>
@@ -21907,15 +21907,15 @@
         <v>17</v>
       </c>
       <c r="C823" s="6">
-        <f>SUM(C824:C835)/SUM(F824:F835)</f>
+        <f>IF(SUM(F824:F835)=0,0,(SUM(C824:C835)/SUM(F824:F835))</f>
         <v/>
       </c>
       <c r="D823" s="6">
-        <f>SUM(D824:D835)/SUM(F824:F835)</f>
+        <f>IF(SUM(F824:F835)=0,0,(SUM(D824:D835)/SUM(F824:F835))</f>
         <v/>
       </c>
       <c r="E823" s="6">
-        <f>SUM(E824:E835)/SUM(F824:F835)</f>
+        <f>IF(SUM(F824:F835)=0,0,(SUM(E824:E835)/SUM(F824:F835))</f>
         <v/>
       </c>
     </row>
@@ -22241,47 +22241,47 @@
         <v>17</v>
       </c>
       <c r="C844" s="6">
-        <f>SUM(C845:C870)/SUM(N845:N870)</f>
+        <f>IF(SUM(N845:N870)=0,0,(SUM(C845:C870)/SUM(N845:N870))</f>
         <v/>
       </c>
       <c r="D844" s="6">
-        <f>SUM(D845:D870)/SUM(N845:N870)</f>
+        <f>IF(SUM(N845:N870)=0,0,(SUM(D845:D870)/SUM(N845:N870))</f>
         <v/>
       </c>
       <c r="E844" s="6">
-        <f>SUM(E845:E870)/SUM(N845:N870)</f>
+        <f>IF(SUM(N845:N870)=0,0,(SUM(E845:E870)/SUM(N845:N870))</f>
         <v/>
       </c>
       <c r="F844" s="6">
-        <f>SUM(F845:F870)/SUM(N845:N870)</f>
+        <f>IF(SUM(N845:N870)=0,0,(SUM(F845:F870)/SUM(N845:N870))</f>
         <v/>
       </c>
       <c r="G844" s="6">
-        <f>SUM(G845:G870)/SUM(N845:N870)</f>
+        <f>IF(SUM(N845:N870)=0,0,(SUM(G845:G870)/SUM(N845:N870))</f>
         <v/>
       </c>
       <c r="H844" s="6">
-        <f>SUM(H845:H870)/SUM(N845:N870)</f>
+        <f>IF(SUM(N845:N870)=0,0,(SUM(H845:H870)/SUM(N845:N870))</f>
         <v/>
       </c>
       <c r="I844" s="6">
-        <f>SUM(I845:I870)/SUM(N845:N870)</f>
+        <f>IF(SUM(N845:N870)=0,0,(SUM(I845:I870)/SUM(N845:N870))</f>
         <v/>
       </c>
       <c r="J844" s="6">
-        <f>SUM(J845:J870)/SUM(N845:N870)</f>
+        <f>IF(SUM(N845:N870)=0,0,(SUM(J845:J870)/SUM(N845:N870))</f>
         <v/>
       </c>
       <c r="K844" s="6">
-        <f>SUM(K845:K870)/SUM(N845:N870)</f>
+        <f>IF(SUM(N845:N870)=0,0,(SUM(K845:K870)/SUM(N845:N870))</f>
         <v/>
       </c>
       <c r="L844" s="6">
-        <f>SUM(L845:L870)/SUM(N845:N870)</f>
+        <f>IF(SUM(N845:N870)=0,0,(SUM(L845:L870)/SUM(N845:N870))</f>
         <v/>
       </c>
       <c r="M844" s="6">
-        <f>SUM(M845:M870)/SUM(N845:N870)</f>
+        <f>IF(SUM(N845:N870)=0,0,(SUM(M845:M870)/SUM(N845:N870))</f>
         <v/>
       </c>
     </row>
@@ -23608,35 +23608,35 @@
         <v>17</v>
       </c>
       <c r="C873" s="6">
-        <f>SUM(C874:C899)/SUM(K874:K899)</f>
+        <f>IF(SUM(K874:K899)=0,0,(SUM(C874:C899)/SUM(K874:K899))</f>
         <v/>
       </c>
       <c r="D873" s="6">
-        <f>SUM(D874:D899)/SUM(K874:K899)</f>
+        <f>IF(SUM(K874:K899)=0,0,(SUM(D874:D899)/SUM(K874:K899))</f>
         <v/>
       </c>
       <c r="E873" s="6">
-        <f>SUM(E874:E899)/SUM(K874:K899)</f>
+        <f>IF(SUM(K874:K899)=0,0,(SUM(E874:E899)/SUM(K874:K899))</f>
         <v/>
       </c>
       <c r="F873" s="6">
-        <f>SUM(F874:F899)/SUM(K874:K899)</f>
+        <f>IF(SUM(K874:K899)=0,0,(SUM(F874:F899)/SUM(K874:K899))</f>
         <v/>
       </c>
       <c r="G873" s="6">
-        <f>SUM(G874:G899)/SUM(K874:K899)</f>
+        <f>IF(SUM(K874:K899)=0,0,(SUM(G874:G899)/SUM(K874:K899))</f>
         <v/>
       </c>
       <c r="H873" s="6">
-        <f>SUM(H874:H899)/SUM(K874:K899)</f>
+        <f>IF(SUM(K874:K899)=0,0,(SUM(H874:H899)/SUM(K874:K899))</f>
         <v/>
       </c>
       <c r="I873" s="6">
-        <f>SUM(I874:I899)/SUM(K874:K899)</f>
+        <f>IF(SUM(K874:K899)=0,0,(SUM(I874:I899)/SUM(K874:K899))</f>
         <v/>
       </c>
       <c r="J873" s="6">
-        <f>SUM(J874:J899)/SUM(K874:K899)</f>
+        <f>IF(SUM(K874:K899)=0,0,(SUM(J874:J899)/SUM(K874:K899))</f>
         <v/>
       </c>
     </row>
@@ -24644,19 +24644,19 @@
         <v>17</v>
       </c>
       <c r="C902" s="6">
-        <f>SUM(C903:C928)/SUM(G903:G928)</f>
+        <f>IF(SUM(G903:G928)=0,0,(SUM(C903:C928)/SUM(G903:G928))</f>
         <v/>
       </c>
       <c r="D902" s="6">
-        <f>SUM(D903:D928)/SUM(G903:G928)</f>
+        <f>IF(SUM(G903:G928)=0,0,(SUM(D903:D928)/SUM(G903:G928))</f>
         <v/>
       </c>
       <c r="E902" s="6">
-        <f>SUM(E903:E928)/SUM(G903:G928)</f>
+        <f>IF(SUM(G903:G928)=0,0,(SUM(E903:E928)/SUM(G903:G928))</f>
         <v/>
       </c>
       <c r="F902" s="6">
-        <f>SUM(F903:F928)/SUM(G903:G928)</f>
+        <f>IF(SUM(G903:G928)=0,0,(SUM(F903:F928)/SUM(G903:G928))</f>
         <v/>
       </c>
     </row>
@@ -25370,47 +25370,47 @@
         <v>17</v>
       </c>
       <c r="C937" s="6">
-        <f>SUM(C938:C969)/SUM(N938:N969)</f>
+        <f>IF(SUM(N938:N969)=0,0,(SUM(C938:C969)/SUM(N938:N969))</f>
         <v/>
       </c>
       <c r="D937" s="6">
-        <f>SUM(D938:D969)/SUM(N938:N969)</f>
+        <f>IF(SUM(N938:N969)=0,0,(SUM(D938:D969)/SUM(N938:N969))</f>
         <v/>
       </c>
       <c r="E937" s="6">
-        <f>SUM(E938:E969)/SUM(N938:N969)</f>
+        <f>IF(SUM(N938:N969)=0,0,(SUM(E938:E969)/SUM(N938:N969))</f>
         <v/>
       </c>
       <c r="F937" s="6">
-        <f>SUM(F938:F969)/SUM(N938:N969)</f>
+        <f>IF(SUM(N938:N969)=0,0,(SUM(F938:F969)/SUM(N938:N969))</f>
         <v/>
       </c>
       <c r="G937" s="6">
-        <f>SUM(G938:G969)/SUM(N938:N969)</f>
+        <f>IF(SUM(N938:N969)=0,0,(SUM(G938:G969)/SUM(N938:N969))</f>
         <v/>
       </c>
       <c r="H937" s="6">
-        <f>SUM(H938:H969)/SUM(N938:N969)</f>
+        <f>IF(SUM(N938:N969)=0,0,(SUM(H938:H969)/SUM(N938:N969))</f>
         <v/>
       </c>
       <c r="I937" s="6">
-        <f>SUM(I938:I969)/SUM(N938:N969)</f>
+        <f>IF(SUM(N938:N969)=0,0,(SUM(I938:I969)/SUM(N938:N969))</f>
         <v/>
       </c>
       <c r="J937" s="6">
-        <f>SUM(J938:J969)/SUM(N938:N969)</f>
+        <f>IF(SUM(N938:N969)=0,0,(SUM(J938:J969)/SUM(N938:N969))</f>
         <v/>
       </c>
       <c r="K937" s="6">
-        <f>SUM(K938:K969)/SUM(N938:N969)</f>
+        <f>IF(SUM(N938:N969)=0,0,(SUM(K938:K969)/SUM(N938:N969))</f>
         <v/>
       </c>
       <c r="L937" s="6">
-        <f>SUM(L938:L969)/SUM(N938:N969)</f>
+        <f>IF(SUM(N938:N969)=0,0,(SUM(L938:L969)/SUM(N938:N969))</f>
         <v/>
       </c>
       <c r="M937" s="6">
-        <f>SUM(M938:M969)/SUM(N938:N969)</f>
+        <f>IF(SUM(N938:N969)=0,0,(SUM(M938:M969)/SUM(N938:N969))</f>
         <v/>
       </c>
     </row>
@@ -27028,35 +27028,35 @@
         <v>17</v>
       </c>
       <c r="C972" s="6">
-        <f>SUM(C973:C1004)/SUM(K973:K1004)</f>
+        <f>IF(SUM(K973:K1004)=0,0,(SUM(C973:C1004)/SUM(K973:K1004))</f>
         <v/>
       </c>
       <c r="D972" s="6">
-        <f>SUM(D973:D1004)/SUM(K973:K1004)</f>
+        <f>IF(SUM(K973:K1004)=0,0,(SUM(D973:D1004)/SUM(K973:K1004))</f>
         <v/>
       </c>
       <c r="E972" s="6">
-        <f>SUM(E973:E1004)/SUM(K973:K1004)</f>
+        <f>IF(SUM(K973:K1004)=0,0,(SUM(E973:E1004)/SUM(K973:K1004))</f>
         <v/>
       </c>
       <c r="F972" s="6">
-        <f>SUM(F973:F1004)/SUM(K973:K1004)</f>
+        <f>IF(SUM(K973:K1004)=0,0,(SUM(F973:F1004)/SUM(K973:K1004))</f>
         <v/>
       </c>
       <c r="G972" s="6">
-        <f>SUM(G973:G1004)/SUM(K973:K1004)</f>
+        <f>IF(SUM(K973:K1004)=0,0,(SUM(G973:G1004)/SUM(K973:K1004))</f>
         <v/>
       </c>
       <c r="H972" s="6">
-        <f>SUM(H973:H1004)/SUM(K973:K1004)</f>
+        <f>IF(SUM(K973:K1004)=0,0,(SUM(H973:H1004)/SUM(K973:K1004))</f>
         <v/>
       </c>
       <c r="I972" s="6">
-        <f>SUM(I973:I1004)/SUM(K973:K1004)</f>
+        <f>IF(SUM(K973:K1004)=0,0,(SUM(I973:I1004)/SUM(K973:K1004))</f>
         <v/>
       </c>
       <c r="J972" s="6">
-        <f>SUM(J973:J1004)/SUM(K973:K1004)</f>
+        <f>IF(SUM(K973:K1004)=0,0,(SUM(J973:J1004)/SUM(K973:K1004))</f>
         <v/>
       </c>
     </row>
@@ -28291,11 +28291,11 @@
         <v>17</v>
       </c>
       <c r="C1007" s="6">
-        <f>SUM(C1008:C1039)/SUM(E1008:E1039)</f>
+        <f>IF(SUM(E1008:E1039)=0,0,(SUM(C1008:C1039)/SUM(E1008:E1039))</f>
         <v/>
       </c>
       <c r="D1007" s="6">
-        <f>SUM(D1008:D1039)/SUM(E1008:E1039)</f>
+        <f>IF(SUM(E1008:E1039)=0,0,(SUM(D1008:D1039)/SUM(E1008:E1039))</f>
         <v/>
       </c>
     </row>
@@ -28969,35 +28969,35 @@
         <v>17</v>
       </c>
       <c r="C1048" s="6">
-        <f>SUM(C1049:C1054)/SUM(K1049:K1054)</f>
+        <f>IF(SUM(K1049:K1054)=0,0,(SUM(C1049:C1054)/SUM(K1049:K1054))</f>
         <v/>
       </c>
       <c r="D1048" s="6">
-        <f>SUM(D1049:D1054)/SUM(K1049:K1054)</f>
+        <f>IF(SUM(K1049:K1054)=0,0,(SUM(D1049:D1054)/SUM(K1049:K1054))</f>
         <v/>
       </c>
       <c r="E1048" s="6">
-        <f>SUM(E1049:E1054)/SUM(K1049:K1054)</f>
+        <f>IF(SUM(K1049:K1054)=0,0,(SUM(E1049:E1054)/SUM(K1049:K1054))</f>
         <v/>
       </c>
       <c r="F1048" s="6">
-        <f>SUM(F1049:F1054)/SUM(K1049:K1054)</f>
+        <f>IF(SUM(K1049:K1054)=0,0,(SUM(F1049:F1054)/SUM(K1049:K1054))</f>
         <v/>
       </c>
       <c r="G1048" s="6">
-        <f>SUM(G1049:G1054)/SUM(K1049:K1054)</f>
+        <f>IF(SUM(K1049:K1054)=0,0,(SUM(G1049:G1054)/SUM(K1049:K1054))</f>
         <v/>
       </c>
       <c r="H1048" s="6">
-        <f>SUM(H1049:H1054)/SUM(K1049:K1054)</f>
+        <f>IF(SUM(K1049:K1054)=0,0,(SUM(H1049:H1054)/SUM(K1049:K1054))</f>
         <v/>
       </c>
       <c r="I1048" s="6">
-        <f>SUM(I1049:I1054)/SUM(K1049:K1054)</f>
+        <f>IF(SUM(K1049:K1054)=0,0,(SUM(I1049:I1054)/SUM(K1049:K1054))</f>
         <v/>
       </c>
       <c r="J1048" s="6">
-        <f>SUM(J1049:J1054)/SUM(K1049:K1054)</f>
+        <f>IF(SUM(K1049:K1054)=0,0,(SUM(J1049:J1054)/SUM(K1049:K1054))</f>
         <v/>
       </c>
     </row>
@@ -29274,23 +29274,23 @@
         <v>17</v>
       </c>
       <c r="C1057" s="6">
-        <f>SUM(C1058:C1063)/SUM(H1058:H1063)</f>
+        <f>IF(SUM(H1058:H1063)=0,0,(SUM(C1058:C1063)/SUM(H1058:H1063))</f>
         <v/>
       </c>
       <c r="D1057" s="6">
-        <f>SUM(D1058:D1063)/SUM(H1058:H1063)</f>
+        <f>IF(SUM(H1058:H1063)=0,0,(SUM(D1058:D1063)/SUM(H1058:H1063))</f>
         <v/>
       </c>
       <c r="E1057" s="6">
-        <f>SUM(E1058:E1063)/SUM(H1058:H1063)</f>
+        <f>IF(SUM(H1058:H1063)=0,0,(SUM(E1058:E1063)/SUM(H1058:H1063))</f>
         <v/>
       </c>
       <c r="F1057" s="6">
-        <f>SUM(F1058:F1063)/SUM(H1058:H1063)</f>
+        <f>IF(SUM(H1058:H1063)=0,0,(SUM(F1058:F1063)/SUM(H1058:H1063))</f>
         <v/>
       </c>
       <c r="G1057" s="6">
-        <f>SUM(G1058:G1063)/SUM(H1058:H1063)</f>
+        <f>IF(SUM(H1058:H1063)=0,0,(SUM(G1058:G1063)/SUM(H1058:H1063))</f>
         <v/>
       </c>
     </row>
@@ -29492,15 +29492,15 @@
         <v>17</v>
       </c>
       <c r="C1066" s="6">
-        <f>SUM(C1067:C1072)/SUM(F1067:F1072)</f>
+        <f>IF(SUM(F1067:F1072)=0,0,(SUM(C1067:C1072)/SUM(F1067:F1072))</f>
         <v/>
       </c>
       <c r="D1066" s="6">
-        <f>SUM(D1067:D1072)/SUM(F1067:F1072)</f>
+        <f>IF(SUM(F1067:F1072)=0,0,(SUM(D1067:D1072)/SUM(F1067:F1072))</f>
         <v/>
       </c>
       <c r="E1066" s="6">
-        <f>SUM(E1067:E1072)/SUM(F1067:F1072)</f>
+        <f>IF(SUM(F1067:F1072)=0,0,(SUM(E1067:E1072)/SUM(F1067:F1072))</f>
         <v/>
       </c>
     </row>
@@ -29676,27 +29676,27 @@
         <v>17</v>
       </c>
       <c r="C1081" s="6">
-        <f>SUM(C1082:C1087)/SUM(I1082:I1087)</f>
+        <f>IF(SUM(I1082:I1087)=0,0,(SUM(C1082:C1087)/SUM(I1082:I1087))</f>
         <v/>
       </c>
       <c r="D1081" s="6">
-        <f>SUM(D1082:D1087)/SUM(I1082:I1087)</f>
+        <f>IF(SUM(I1082:I1087)=0,0,(SUM(D1082:D1087)/SUM(I1082:I1087))</f>
         <v/>
       </c>
       <c r="E1081" s="6">
-        <f>SUM(E1082:E1087)/SUM(I1082:I1087)</f>
+        <f>IF(SUM(I1082:I1087)=0,0,(SUM(E1082:E1087)/SUM(I1082:I1087))</f>
         <v/>
       </c>
       <c r="F1081" s="6">
-        <f>SUM(F1082:F1087)/SUM(I1082:I1087)</f>
+        <f>IF(SUM(I1082:I1087)=0,0,(SUM(F1082:F1087)/SUM(I1082:I1087))</f>
         <v/>
       </c>
       <c r="G1081" s="6">
-        <f>SUM(G1082:G1087)/SUM(I1082:I1087)</f>
+        <f>IF(SUM(I1082:I1087)=0,0,(SUM(G1082:G1087)/SUM(I1082:I1087))</f>
         <v/>
       </c>
       <c r="H1081" s="6">
-        <f>SUM(H1082:H1087)/SUM(I1082:I1087)</f>
+        <f>IF(SUM(I1082:I1087)=0,0,(SUM(H1082:H1087)/SUM(I1082:I1087))</f>
         <v/>
       </c>
     </row>
@@ -29928,11 +29928,11 @@
         <v>17</v>
       </c>
       <c r="C1090" s="6">
-        <f>SUM(C1091:C1096)/SUM(E1091:E1096)</f>
+        <f>IF(SUM(E1091:E1096)=0,0,(SUM(C1091:C1096)/SUM(E1091:E1096))</f>
         <v/>
       </c>
       <c r="D1090" s="6">
-        <f>SUM(D1091:D1096)/SUM(E1091:E1096)</f>
+        <f>IF(SUM(E1091:E1096)=0,0,(SUM(D1091:D1096)/SUM(E1091:E1096))</f>
         <v/>
       </c>
     </row>
@@ -30073,7 +30073,7 @@
         <v>17</v>
       </c>
       <c r="C1099" s="6">
-        <f>SUM(C1100:C1105)/SUM(D1100:D1105)</f>
+        <f>IF(SUM(D1100:D1105)=0,0,(SUM(C1100:C1105)/SUM(D1100:D1105))</f>
         <v/>
       </c>
     </row>
@@ -30227,47 +30227,47 @@
         <v>17</v>
       </c>
       <c r="C1114" s="6">
-        <f>SUM(C1115:C1131)/SUM(N1115:N1131)</f>
+        <f>IF(SUM(N1115:N1131)=0,0,(SUM(C1115:C1131)/SUM(N1115:N1131))</f>
         <v/>
       </c>
       <c r="D1114" s="6">
-        <f>SUM(D1115:D1131)/SUM(N1115:N1131)</f>
+        <f>IF(SUM(N1115:N1131)=0,0,(SUM(D1115:D1131)/SUM(N1115:N1131))</f>
         <v/>
       </c>
       <c r="E1114" s="6">
-        <f>SUM(E1115:E1131)/SUM(N1115:N1131)</f>
+        <f>IF(SUM(N1115:N1131)=0,0,(SUM(E1115:E1131)/SUM(N1115:N1131))</f>
         <v/>
       </c>
       <c r="F1114" s="6">
-        <f>SUM(F1115:F1131)/SUM(N1115:N1131)</f>
+        <f>IF(SUM(N1115:N1131)=0,0,(SUM(F1115:F1131)/SUM(N1115:N1131))</f>
         <v/>
       </c>
       <c r="G1114" s="6">
-        <f>SUM(G1115:G1131)/SUM(N1115:N1131)</f>
+        <f>IF(SUM(N1115:N1131)=0,0,(SUM(G1115:G1131)/SUM(N1115:N1131))</f>
         <v/>
       </c>
       <c r="H1114" s="6">
-        <f>SUM(H1115:H1131)/SUM(N1115:N1131)</f>
+        <f>IF(SUM(N1115:N1131)=0,0,(SUM(H1115:H1131)/SUM(N1115:N1131))</f>
         <v/>
       </c>
       <c r="I1114" s="6">
-        <f>SUM(I1115:I1131)/SUM(N1115:N1131)</f>
+        <f>IF(SUM(N1115:N1131)=0,0,(SUM(I1115:I1131)/SUM(N1115:N1131))</f>
         <v/>
       </c>
       <c r="J1114" s="6">
-        <f>SUM(J1115:J1131)/SUM(N1115:N1131)</f>
+        <f>IF(SUM(N1115:N1131)=0,0,(SUM(J1115:J1131)/SUM(N1115:N1131))</f>
         <v/>
       </c>
       <c r="K1114" s="6">
-        <f>SUM(K1115:K1131)/SUM(N1115:N1131)</f>
+        <f>IF(SUM(N1115:N1131)=0,0,(SUM(K1115:K1131)/SUM(N1115:N1131))</f>
         <v/>
       </c>
       <c r="L1114" s="6">
-        <f>SUM(L1115:L1131)/SUM(N1115:N1131)</f>
+        <f>IF(SUM(N1115:N1131)=0,0,(SUM(L1115:L1131)/SUM(N1115:N1131))</f>
         <v/>
       </c>
       <c r="M1114" s="6">
-        <f>SUM(M1115:M1131)/SUM(N1115:N1131)</f>
+        <f>IF(SUM(N1115:N1131)=0,0,(SUM(M1115:M1131)/SUM(N1115:N1131))</f>
         <v/>
       </c>
     </row>
@@ -31152,31 +31152,31 @@
         <v>17</v>
       </c>
       <c r="C1134" s="6">
-        <f>SUM(C1135:C1151)/SUM(J1135:J1151)</f>
+        <f>IF(SUM(J1135:J1151)=0,0,(SUM(C1135:C1151)/SUM(J1135:J1151))</f>
         <v/>
       </c>
       <c r="D1134" s="6">
-        <f>SUM(D1135:D1151)/SUM(J1135:J1151)</f>
+        <f>IF(SUM(J1135:J1151)=0,0,(SUM(D1135:D1151)/SUM(J1135:J1151))</f>
         <v/>
       </c>
       <c r="E1134" s="6">
-        <f>SUM(E1135:E1151)/SUM(J1135:J1151)</f>
+        <f>IF(SUM(J1135:J1151)=0,0,(SUM(E1135:E1151)/SUM(J1135:J1151))</f>
         <v/>
       </c>
       <c r="F1134" s="6">
-        <f>SUM(F1135:F1151)/SUM(J1135:J1151)</f>
+        <f>IF(SUM(J1135:J1151)=0,0,(SUM(F1135:F1151)/SUM(J1135:J1151))</f>
         <v/>
       </c>
       <c r="G1134" s="6">
-        <f>SUM(G1135:G1151)/SUM(J1135:J1151)</f>
+        <f>IF(SUM(J1135:J1151)=0,0,(SUM(G1135:G1151)/SUM(J1135:J1151))</f>
         <v/>
       </c>
       <c r="H1134" s="6">
-        <f>SUM(H1135:H1151)/SUM(J1135:J1151)</f>
+        <f>IF(SUM(J1135:J1151)=0,0,(SUM(H1135:H1151)/SUM(J1135:J1151))</f>
         <v/>
       </c>
       <c r="I1134" s="6">
-        <f>SUM(I1135:I1151)/SUM(J1135:J1151)</f>
+        <f>IF(SUM(J1135:J1151)=0,0,(SUM(I1135:I1151)/SUM(J1135:J1151))</f>
         <v/>
       </c>
     </row>
@@ -31795,15 +31795,15 @@
         <v>17</v>
       </c>
       <c r="C1154" s="6">
-        <f>SUM(C1155:C1171)/SUM(F1155:F1171)</f>
+        <f>IF(SUM(F1155:F1171)=0,0,(SUM(C1155:C1171)/SUM(F1155:F1171))</f>
         <v/>
       </c>
       <c r="D1154" s="6">
-        <f>SUM(D1155:D1171)/SUM(F1155:F1171)</f>
+        <f>IF(SUM(F1155:F1171)=0,0,(SUM(D1155:D1171)/SUM(F1155:F1171))</f>
         <v/>
       </c>
       <c r="E1154" s="6">
-        <f>SUM(E1155:E1171)/SUM(F1155:F1171)</f>
+        <f>IF(SUM(F1155:F1171)=0,0,(SUM(E1155:E1171)/SUM(F1155:F1171))</f>
         <v/>
       </c>
     </row>
@@ -32231,39 +32231,39 @@
         <v>17</v>
       </c>
       <c r="C1180" s="6">
-        <f>SUM(C1181:C1200)/SUM(L1181:L1200)</f>
+        <f>IF(SUM(L1181:L1200)=0,0,(SUM(C1181:C1200)/SUM(L1181:L1200))</f>
         <v/>
       </c>
       <c r="D1180" s="6">
-        <f>SUM(D1181:D1200)/SUM(L1181:L1200)</f>
+        <f>IF(SUM(L1181:L1200)=0,0,(SUM(D1181:D1200)/SUM(L1181:L1200))</f>
         <v/>
       </c>
       <c r="E1180" s="6">
-        <f>SUM(E1181:E1200)/SUM(L1181:L1200)</f>
+        <f>IF(SUM(L1181:L1200)=0,0,(SUM(E1181:E1200)/SUM(L1181:L1200))</f>
         <v/>
       </c>
       <c r="F1180" s="6">
-        <f>SUM(F1181:F1200)/SUM(L1181:L1200)</f>
+        <f>IF(SUM(L1181:L1200)=0,0,(SUM(F1181:F1200)/SUM(L1181:L1200))</f>
         <v/>
       </c>
       <c r="G1180" s="6">
-        <f>SUM(G1181:G1200)/SUM(L1181:L1200)</f>
+        <f>IF(SUM(L1181:L1200)=0,0,(SUM(G1181:G1200)/SUM(L1181:L1200))</f>
         <v/>
       </c>
       <c r="H1180" s="6">
-        <f>SUM(H1181:H1200)/SUM(L1181:L1200)</f>
+        <f>IF(SUM(L1181:L1200)=0,0,(SUM(H1181:H1200)/SUM(L1181:L1200))</f>
         <v/>
       </c>
       <c r="I1180" s="6">
-        <f>SUM(I1181:I1200)/SUM(L1181:L1200)</f>
+        <f>IF(SUM(L1181:L1200)=0,0,(SUM(I1181:I1200)/SUM(L1181:L1200))</f>
         <v/>
       </c>
       <c r="J1180" s="6">
-        <f>SUM(J1181:J1200)/SUM(L1181:L1200)</f>
+        <f>IF(SUM(L1181:L1200)=0,0,(SUM(J1181:J1200)/SUM(L1181:L1200))</f>
         <v/>
       </c>
       <c r="K1180" s="6">
-        <f>SUM(K1181:K1200)/SUM(L1181:L1200)</f>
+        <f>IF(SUM(L1181:L1200)=0,0,(SUM(K1181:K1200)/SUM(L1181:L1200))</f>
         <v/>
       </c>
     </row>
@@ -33160,23 +33160,23 @@
         <v>17</v>
       </c>
       <c r="C1203" s="6">
-        <f>SUM(C1204:C1223)/SUM(H1204:H1223)</f>
+        <f>IF(SUM(H1204:H1223)=0,0,(SUM(C1204:C1223)/SUM(H1204:H1223))</f>
         <v/>
       </c>
       <c r="D1203" s="6">
-        <f>SUM(D1204:D1223)/SUM(H1204:H1223)</f>
+        <f>IF(SUM(H1204:H1223)=0,0,(SUM(D1204:D1223)/SUM(H1204:H1223))</f>
         <v/>
       </c>
       <c r="E1203" s="6">
-        <f>SUM(E1204:E1223)/SUM(H1204:H1223)</f>
+        <f>IF(SUM(H1204:H1223)=0,0,(SUM(E1204:E1223)/SUM(H1204:H1223))</f>
         <v/>
       </c>
       <c r="F1203" s="6">
-        <f>SUM(F1204:F1223)/SUM(H1204:H1223)</f>
+        <f>IF(SUM(H1204:H1223)=0,0,(SUM(F1204:F1223)/SUM(H1204:H1223))</f>
         <v/>
       </c>
       <c r="G1203" s="6">
-        <f>SUM(G1204:G1223)/SUM(H1204:H1223)</f>
+        <f>IF(SUM(H1204:H1223)=0,0,(SUM(G1204:G1223)/SUM(H1204:H1223))</f>
         <v/>
       </c>
     </row>
@@ -33786,19 +33786,19 @@
         <v>17</v>
       </c>
       <c r="C1226" s="6">
-        <f>SUM(C1227:C1246)/SUM(G1227:G1246)</f>
+        <f>IF(SUM(G1227:G1246)=0,0,(SUM(C1227:C1246)/SUM(G1227:G1246))</f>
         <v/>
       </c>
       <c r="D1226" s="6">
-        <f>SUM(D1227:D1246)/SUM(G1227:G1246)</f>
+        <f>IF(SUM(G1227:G1246)=0,0,(SUM(D1227:D1246)/SUM(G1227:G1246))</f>
         <v/>
       </c>
       <c r="E1226" s="6">
-        <f>SUM(E1227:E1246)/SUM(G1227:G1246)</f>
+        <f>IF(SUM(G1227:G1246)=0,0,(SUM(E1227:E1246)/SUM(G1227:G1246))</f>
         <v/>
       </c>
       <c r="F1226" s="6">
-        <f>SUM(F1227:F1246)/SUM(G1227:G1246)</f>
+        <f>IF(SUM(G1227:G1246)=0,0,(SUM(F1227:F1246)/SUM(G1227:G1246))</f>
         <v/>
       </c>
     </row>
@@ -34354,27 +34354,27 @@
         <v>17</v>
       </c>
       <c r="C1255" s="6">
-        <f>SUM(C1256:C1262)/SUM(I1256:I1262)</f>
+        <f>IF(SUM(I1256:I1262)=0,0,(SUM(C1256:C1262)/SUM(I1256:I1262))</f>
         <v/>
       </c>
       <c r="D1255" s="6">
-        <f>SUM(D1256:D1262)/SUM(I1256:I1262)</f>
+        <f>IF(SUM(I1256:I1262)=0,0,(SUM(D1256:D1262)/SUM(I1256:I1262))</f>
         <v/>
       </c>
       <c r="E1255" s="6">
-        <f>SUM(E1256:E1262)/SUM(I1256:I1262)</f>
+        <f>IF(SUM(I1256:I1262)=0,0,(SUM(E1256:E1262)/SUM(I1256:I1262))</f>
         <v/>
       </c>
       <c r="F1255" s="6">
-        <f>SUM(F1256:F1262)/SUM(I1256:I1262)</f>
+        <f>IF(SUM(I1256:I1262)=0,0,(SUM(F1256:F1262)/SUM(I1256:I1262))</f>
         <v/>
       </c>
       <c r="G1255" s="6">
-        <f>SUM(G1256:G1262)/SUM(I1256:I1262)</f>
+        <f>IF(SUM(I1256:I1262)=0,0,(SUM(G1256:G1262)/SUM(I1256:I1262))</f>
         <v/>
       </c>
       <c r="H1255" s="6">
-        <f>SUM(H1256:H1262)/SUM(I1256:I1262)</f>
+        <f>IF(SUM(I1256:I1262)=0,0,(SUM(H1256:H1262)/SUM(I1256:I1262))</f>
         <v/>
       </c>
     </row>
@@ -34642,15 +34642,15 @@
         <v>17</v>
       </c>
       <c r="C1265" s="6">
-        <f>SUM(C1266:C1272)/SUM(F1266:F1272)</f>
+        <f>IF(SUM(F1266:F1272)=0,0,(SUM(C1266:C1272)/SUM(F1266:F1272))</f>
         <v/>
       </c>
       <c r="D1265" s="6">
-        <f>SUM(D1266:D1272)/SUM(F1266:F1272)</f>
+        <f>IF(SUM(F1266:F1272)=0,0,(SUM(D1266:D1272)/SUM(F1266:F1272))</f>
         <v/>
       </c>
       <c r="E1265" s="6">
-        <f>SUM(E1266:E1272)/SUM(F1266:F1272)</f>
+        <f>IF(SUM(F1266:F1272)=0,0,(SUM(E1266:E1272)/SUM(F1266:F1272))</f>
         <v/>
       </c>
     </row>
@@ -34834,11 +34834,11 @@
         <v>17</v>
       </c>
       <c r="C1275" s="6">
-        <f>SUM(C1276:C1282)/SUM(E1276:E1282)</f>
+        <f>IF(SUM(E1276:E1282)=0,0,(SUM(C1276:C1282)/SUM(E1276:E1282))</f>
         <v/>
       </c>
       <c r="D1275" s="6">
-        <f>SUM(D1276:D1282)/SUM(E1276:E1282)</f>
+        <f>IF(SUM(E1276:E1282)=0,0,(SUM(D1276:D1282)/SUM(E1276:E1282))</f>
         <v/>
       </c>
     </row>
@@ -35017,31 +35017,31 @@
         <v>17</v>
       </c>
       <c r="C1291" s="6">
-        <f>SUM(C1292:C1309)/SUM(J1292:J1309)</f>
+        <f>IF(SUM(J1292:J1309)=0,0,(SUM(C1292:C1309)/SUM(J1292:J1309))</f>
         <v/>
       </c>
       <c r="D1291" s="6">
-        <f>SUM(D1292:D1309)/SUM(J1292:J1309)</f>
+        <f>IF(SUM(J1292:J1309)=0,0,(SUM(D1292:D1309)/SUM(J1292:J1309))</f>
         <v/>
       </c>
       <c r="E1291" s="6">
-        <f>SUM(E1292:E1309)/SUM(J1292:J1309)</f>
+        <f>IF(SUM(J1292:J1309)=0,0,(SUM(E1292:E1309)/SUM(J1292:J1309))</f>
         <v/>
       </c>
       <c r="F1291" s="6">
-        <f>SUM(F1292:F1309)/SUM(J1292:J1309)</f>
+        <f>IF(SUM(J1292:J1309)=0,0,(SUM(F1292:F1309)/SUM(J1292:J1309))</f>
         <v/>
       </c>
       <c r="G1291" s="6">
-        <f>SUM(G1292:G1309)/SUM(J1292:J1309)</f>
+        <f>IF(SUM(J1292:J1309)=0,0,(SUM(G1292:G1309)/SUM(J1292:J1309))</f>
         <v/>
       </c>
       <c r="H1291" s="6">
-        <f>SUM(H1292:H1309)/SUM(J1292:J1309)</f>
+        <f>IF(SUM(J1292:J1309)=0,0,(SUM(H1292:H1309)/SUM(J1292:J1309))</f>
         <v/>
       </c>
       <c r="I1291" s="6">
-        <f>SUM(I1292:I1309)/SUM(J1292:J1309)</f>
+        <f>IF(SUM(J1292:J1309)=0,0,(SUM(I1292:I1309)/SUM(J1292:J1309))</f>
         <v/>
       </c>
     </row>
@@ -35754,39 +35754,39 @@
         <v>17</v>
       </c>
       <c r="C1312" s="6">
-        <f>SUM(C1313:C1330)/SUM(L1313:L1330)</f>
+        <f>IF(SUM(L1313:L1330)=0,0,(SUM(C1313:C1330)/SUM(L1313:L1330))</f>
         <v/>
       </c>
       <c r="D1312" s="6">
-        <f>SUM(D1313:D1330)/SUM(L1313:L1330)</f>
+        <f>IF(SUM(L1313:L1330)=0,0,(SUM(D1313:D1330)/SUM(L1313:L1330))</f>
         <v/>
       </c>
       <c r="E1312" s="6">
-        <f>SUM(E1313:E1330)/SUM(L1313:L1330)</f>
+        <f>IF(SUM(L1313:L1330)=0,0,(SUM(E1313:E1330)/SUM(L1313:L1330))</f>
         <v/>
       </c>
       <c r="F1312" s="6">
-        <f>SUM(F1313:F1330)/SUM(L1313:L1330)</f>
+        <f>IF(SUM(L1313:L1330)=0,0,(SUM(F1313:F1330)/SUM(L1313:L1330))</f>
         <v/>
       </c>
       <c r="G1312" s="6">
-        <f>SUM(G1313:G1330)/SUM(L1313:L1330)</f>
+        <f>IF(SUM(L1313:L1330)=0,0,(SUM(G1313:G1330)/SUM(L1313:L1330))</f>
         <v/>
       </c>
       <c r="H1312" s="6">
-        <f>SUM(H1313:H1330)/SUM(L1313:L1330)</f>
+        <f>IF(SUM(L1313:L1330)=0,0,(SUM(H1313:H1330)/SUM(L1313:L1330))</f>
         <v/>
       </c>
       <c r="I1312" s="6">
-        <f>SUM(I1313:I1330)/SUM(L1313:L1330)</f>
+        <f>IF(SUM(L1313:L1330)=0,0,(SUM(I1313:I1330)/SUM(L1313:L1330))</f>
         <v/>
       </c>
       <c r="J1312" s="6">
-        <f>SUM(J1313:J1330)/SUM(L1313:L1330)</f>
+        <f>IF(SUM(L1313:L1330)=0,0,(SUM(J1313:J1330)/SUM(L1313:L1330))</f>
         <v/>
       </c>
       <c r="K1312" s="6">
-        <f>SUM(K1313:K1330)/SUM(L1313:L1330)</f>
+        <f>IF(SUM(L1313:L1330)=0,0,(SUM(K1313:K1330)/SUM(L1313:L1330))</f>
         <v/>
       </c>
     </row>
@@ -36550,15 +36550,15 @@
         <v>17</v>
       </c>
       <c r="C1333" s="6">
-        <f>SUM(C1334:C1351)/SUM(F1334:F1351)</f>
+        <f>IF(SUM(F1334:F1351)=0,0,(SUM(C1334:C1351)/SUM(F1334:F1351))</f>
         <v/>
       </c>
       <c r="D1333" s="6">
-        <f>SUM(D1334:D1351)/SUM(F1334:F1351)</f>
+        <f>IF(SUM(F1334:F1351)=0,0,(SUM(D1334:D1351)/SUM(F1334:F1351))</f>
         <v/>
       </c>
       <c r="E1333" s="6">
-        <f>SUM(E1334:E1351)/SUM(F1334:F1351)</f>
+        <f>IF(SUM(F1334:F1351)=0,0,(SUM(E1334:E1351)/SUM(F1334:F1351))</f>
         <v/>
       </c>
     </row>
@@ -36993,19 +36993,19 @@
         <v>17</v>
       </c>
       <c r="C1360" s="6">
-        <f>SUM(C1361:C1364)/SUM(G1361:G1364)</f>
+        <f>IF(SUM(G1361:G1364)=0,0,(SUM(C1361:C1364)/SUM(G1361:G1364))</f>
         <v/>
       </c>
       <c r="D1360" s="6">
-        <f>SUM(D1361:D1364)/SUM(G1361:G1364)</f>
+        <f>IF(SUM(G1361:G1364)=0,0,(SUM(D1361:D1364)/SUM(G1361:G1364))</f>
         <v/>
       </c>
       <c r="E1360" s="6">
-        <f>SUM(E1361:E1364)/SUM(G1361:G1364)</f>
+        <f>IF(SUM(G1361:G1364)=0,0,(SUM(E1361:E1364)/SUM(G1361:G1364))</f>
         <v/>
       </c>
       <c r="F1360" s="6">
-        <f>SUM(F1361:F1364)/SUM(G1361:G1364)</f>
+        <f>IF(SUM(G1361:G1364)=0,0,(SUM(F1361:F1364)/SUM(G1361:G1364))</f>
         <v/>
       </c>
     </row>
@@ -37152,23 +37152,23 @@
         <v>17</v>
       </c>
       <c r="C1367" s="6">
-        <f>SUM(C1368:C1371)/SUM(H1368:H1371)</f>
+        <f>IF(SUM(H1368:H1371)=0,0,(SUM(C1368:C1371)/SUM(H1368:H1371))</f>
         <v/>
       </c>
       <c r="D1367" s="6">
-        <f>SUM(D1368:D1371)/SUM(H1368:H1371)</f>
+        <f>IF(SUM(H1368:H1371)=0,0,(SUM(D1368:D1371)/SUM(H1368:H1371))</f>
         <v/>
       </c>
       <c r="E1367" s="6">
-        <f>SUM(E1368:E1371)/SUM(H1368:H1371)</f>
+        <f>IF(SUM(H1368:H1371)=0,0,(SUM(E1368:E1371)/SUM(H1368:H1371))</f>
         <v/>
       </c>
       <c r="F1367" s="6">
-        <f>SUM(F1368:F1371)/SUM(H1368:H1371)</f>
+        <f>IF(SUM(H1368:H1371)=0,0,(SUM(F1368:F1371)/SUM(H1368:H1371))</f>
         <v/>
       </c>
       <c r="G1367" s="6">
-        <f>SUM(G1368:G1371)/SUM(H1368:H1371)</f>
+        <f>IF(SUM(H1368:H1371)=0,0,(SUM(G1368:G1371)/SUM(H1368:H1371))</f>
         <v/>
       </c>
     </row>
@@ -37306,7 +37306,7 @@
         <v>17</v>
       </c>
       <c r="C1374" s="6">
-        <f>SUM(C1375:C1378)/SUM(D1375:D1378)</f>
+        <f>IF(SUM(D1375:D1378)=0,0,(SUM(C1375:C1378)/SUM(D1375:D1378))</f>
         <v/>
       </c>
     </row>
@@ -37419,35 +37419,35 @@
         <v>17</v>
       </c>
       <c r="C1387" s="6">
-        <f>SUM(C1388:C1408)/SUM(K1388:K1408)</f>
+        <f>IF(SUM(K1388:K1408)=0,0,(SUM(C1388:C1408)/SUM(K1388:K1408))</f>
         <v/>
       </c>
       <c r="D1387" s="6">
-        <f>SUM(D1388:D1408)/SUM(K1388:K1408)</f>
+        <f>IF(SUM(K1388:K1408)=0,0,(SUM(D1388:D1408)/SUM(K1388:K1408))</f>
         <v/>
       </c>
       <c r="E1387" s="6">
-        <f>SUM(E1388:E1408)/SUM(K1388:K1408)</f>
+        <f>IF(SUM(K1388:K1408)=0,0,(SUM(E1388:E1408)/SUM(K1388:K1408))</f>
         <v/>
       </c>
       <c r="F1387" s="6">
-        <f>SUM(F1388:F1408)/SUM(K1388:K1408)</f>
+        <f>IF(SUM(K1388:K1408)=0,0,(SUM(F1388:F1408)/SUM(K1388:K1408))</f>
         <v/>
       </c>
       <c r="G1387" s="6">
-        <f>SUM(G1388:G1408)/SUM(K1388:K1408)</f>
+        <f>IF(SUM(K1388:K1408)=0,0,(SUM(G1388:G1408)/SUM(K1388:K1408))</f>
         <v/>
       </c>
       <c r="H1387" s="6">
-        <f>SUM(H1388:H1408)/SUM(K1388:K1408)</f>
+        <f>IF(SUM(K1388:K1408)=0,0,(SUM(H1388:H1408)/SUM(K1388:K1408))</f>
         <v/>
       </c>
       <c r="I1387" s="6">
-        <f>SUM(I1388:I1408)/SUM(K1388:K1408)</f>
+        <f>IF(SUM(K1388:K1408)=0,0,(SUM(I1388:I1408)/SUM(K1388:K1408))</f>
         <v/>
       </c>
       <c r="J1387" s="6">
-        <f>SUM(J1388:J1408)/SUM(K1388:K1408)</f>
+        <f>IF(SUM(K1388:K1408)=0,0,(SUM(J1388:J1408)/SUM(K1388:K1408))</f>
         <v/>
       </c>
     </row>
@@ -38334,35 +38334,35 @@
         <v>17</v>
       </c>
       <c r="C1411" s="6">
-        <f>SUM(C1412:C1432)/SUM(K1412:K1432)</f>
+        <f>IF(SUM(K1412:K1432)=0,0,(SUM(C1412:C1432)/SUM(K1412:K1432))</f>
         <v/>
       </c>
       <c r="D1411" s="6">
-        <f>SUM(D1412:D1432)/SUM(K1412:K1432)</f>
+        <f>IF(SUM(K1412:K1432)=0,0,(SUM(D1412:D1432)/SUM(K1412:K1432))</f>
         <v/>
       </c>
       <c r="E1411" s="6">
-        <f>SUM(E1412:E1432)/SUM(K1412:K1432)</f>
+        <f>IF(SUM(K1412:K1432)=0,0,(SUM(E1412:E1432)/SUM(K1412:K1432))</f>
         <v/>
       </c>
       <c r="F1411" s="6">
-        <f>SUM(F1412:F1432)/SUM(K1412:K1432)</f>
+        <f>IF(SUM(K1412:K1432)=0,0,(SUM(F1412:F1432)/SUM(K1412:K1432))</f>
         <v/>
       </c>
       <c r="G1411" s="6">
-        <f>SUM(G1412:G1432)/SUM(K1412:K1432)</f>
+        <f>IF(SUM(K1412:K1432)=0,0,(SUM(G1412:G1432)/SUM(K1412:K1432))</f>
         <v/>
       </c>
       <c r="H1411" s="6">
-        <f>SUM(H1412:H1432)/SUM(K1412:K1432)</f>
+        <f>IF(SUM(K1412:K1432)=0,0,(SUM(H1412:H1432)/SUM(K1412:K1432))</f>
         <v/>
       </c>
       <c r="I1411" s="6">
-        <f>SUM(I1412:I1432)/SUM(K1412:K1432)</f>
+        <f>IF(SUM(K1412:K1432)=0,0,(SUM(I1412:I1432)/SUM(K1412:K1432))</f>
         <v/>
       </c>
       <c r="J1411" s="6">
-        <f>SUM(J1412:J1432)/SUM(K1412:K1432)</f>
+        <f>IF(SUM(K1412:K1432)=0,0,(SUM(J1412:J1432)/SUM(K1412:K1432))</f>
         <v/>
       </c>
     </row>
@@ -39187,15 +39187,15 @@
         <v>17</v>
       </c>
       <c r="C1435" s="6">
-        <f>SUM(C1436:C1456)/SUM(F1436:F1456)</f>
+        <f>IF(SUM(F1436:F1456)=0,0,(SUM(C1436:C1456)/SUM(F1436:F1456))</f>
         <v/>
       </c>
       <c r="D1435" s="6">
-        <f>SUM(D1436:D1456)/SUM(F1436:F1456)</f>
+        <f>IF(SUM(F1436:F1456)=0,0,(SUM(D1436:D1456)/SUM(F1436:F1456))</f>
         <v/>
       </c>
       <c r="E1435" s="6">
-        <f>SUM(E1436:E1456)/SUM(F1436:F1456)</f>
+        <f>IF(SUM(F1436:F1456)=0,0,(SUM(E1436:E1456)/SUM(F1436:F1456))</f>
         <v/>
       </c>
     </row>
@@ -39712,39 +39712,39 @@
         <v>17</v>
       </c>
       <c r="C1465" s="6">
-        <f>SUM(C1466:C1475)/SUM(L1466:L1475)</f>
+        <f>IF(SUM(L1466:L1475)=0,0,(SUM(C1466:C1475)/SUM(L1466:L1475))</f>
         <v/>
       </c>
       <c r="D1465" s="6">
-        <f>SUM(D1466:D1475)/SUM(L1466:L1475)</f>
+        <f>IF(SUM(L1466:L1475)=0,0,(SUM(D1466:D1475)/SUM(L1466:L1475))</f>
         <v/>
       </c>
       <c r="E1465" s="6">
-        <f>SUM(E1466:E1475)/SUM(L1466:L1475)</f>
+        <f>IF(SUM(L1466:L1475)=0,0,(SUM(E1466:E1475)/SUM(L1466:L1475))</f>
         <v/>
       </c>
       <c r="F1465" s="6">
-        <f>SUM(F1466:F1475)/SUM(L1466:L1475)</f>
+        <f>IF(SUM(L1466:L1475)=0,0,(SUM(F1466:F1475)/SUM(L1466:L1475))</f>
         <v/>
       </c>
       <c r="G1465" s="6">
-        <f>SUM(G1466:G1475)/SUM(L1466:L1475)</f>
+        <f>IF(SUM(L1466:L1475)=0,0,(SUM(G1466:G1475)/SUM(L1466:L1475))</f>
         <v/>
       </c>
       <c r="H1465" s="6">
-        <f>SUM(H1466:H1475)/SUM(L1466:L1475)</f>
+        <f>IF(SUM(L1466:L1475)=0,0,(SUM(H1466:H1475)/SUM(L1466:L1475))</f>
         <v/>
       </c>
       <c r="I1465" s="6">
-        <f>SUM(I1466:I1475)/SUM(L1466:L1475)</f>
+        <f>IF(SUM(L1466:L1475)=0,0,(SUM(I1466:I1475)/SUM(L1466:L1475))</f>
         <v/>
       </c>
       <c r="J1465" s="6">
-        <f>SUM(J1466:J1475)/SUM(L1466:L1475)</f>
+        <f>IF(SUM(L1466:L1475)=0,0,(SUM(J1466:J1475)/SUM(L1466:L1475))</f>
         <v/>
       </c>
       <c r="K1465" s="6">
-        <f>SUM(K1466:K1475)/SUM(L1466:L1475)</f>
+        <f>IF(SUM(L1466:L1475)=0,0,(SUM(K1466:K1475)/SUM(L1466:L1475))</f>
         <v/>
       </c>
     </row>
@@ -40210,23 +40210,23 @@
         <v>17</v>
       </c>
       <c r="C1478" s="6">
-        <f>SUM(C1479:C1488)/SUM(H1479:H1488)</f>
+        <f>IF(SUM(H1479:H1488)=0,0,(SUM(C1479:C1488)/SUM(H1479:H1488))</f>
         <v/>
       </c>
       <c r="D1478" s="6">
-        <f>SUM(D1479:D1488)/SUM(H1479:H1488)</f>
+        <f>IF(SUM(H1479:H1488)=0,0,(SUM(D1479:D1488)/SUM(H1479:H1488))</f>
         <v/>
       </c>
       <c r="E1478" s="6">
-        <f>SUM(E1479:E1488)/SUM(H1479:H1488)</f>
+        <f>IF(SUM(H1479:H1488)=0,0,(SUM(E1479:E1488)/SUM(H1479:H1488))</f>
         <v/>
       </c>
       <c r="F1478" s="6">
-        <f>SUM(F1479:F1488)/SUM(H1479:H1488)</f>
+        <f>IF(SUM(H1479:H1488)=0,0,(SUM(F1479:F1488)/SUM(H1479:H1488))</f>
         <v/>
       </c>
       <c r="G1478" s="6">
-        <f>SUM(G1479:G1488)/SUM(H1479:H1488)</f>
+        <f>IF(SUM(H1479:H1488)=0,0,(SUM(G1479:G1488)/SUM(H1479:H1488))</f>
         <v/>
       </c>
     </row>
@@ -40536,11 +40536,11 @@
         <v>17</v>
       </c>
       <c r="C1491" s="6">
-        <f>SUM(C1492:C1501)/SUM(E1492:E1501)</f>
+        <f>IF(SUM(E1492:E1501)=0,0,(SUM(C1492:C1501)/SUM(E1492:E1501))</f>
         <v/>
       </c>
       <c r="D1491" s="6">
-        <f>SUM(D1492:D1501)/SUM(E1492:E1501)</f>
+        <f>IF(SUM(E1492:E1501)=0,0,(SUM(D1492:D1501)/SUM(E1492:E1501))</f>
         <v/>
       </c>
     </row>
@@ -40789,47 +40789,47 @@
         <v>17</v>
       </c>
       <c r="C1510" s="6">
-        <f>SUM(C1511:C1519)/SUM(N1511:N1519)</f>
+        <f>IF(SUM(N1511:N1519)=0,0,(SUM(C1511:C1519)/SUM(N1511:N1519))</f>
         <v/>
       </c>
       <c r="D1510" s="6">
-        <f>SUM(D1511:D1519)/SUM(N1511:N1519)</f>
+        <f>IF(SUM(N1511:N1519)=0,0,(SUM(D1511:D1519)/SUM(N1511:N1519))</f>
         <v/>
       </c>
       <c r="E1510" s="6">
-        <f>SUM(E1511:E1519)/SUM(N1511:N1519)</f>
+        <f>IF(SUM(N1511:N1519)=0,0,(SUM(E1511:E1519)/SUM(N1511:N1519))</f>
         <v/>
       </c>
       <c r="F1510" s="6">
-        <f>SUM(F1511:F1519)/SUM(N1511:N1519)</f>
+        <f>IF(SUM(N1511:N1519)=0,0,(SUM(F1511:F1519)/SUM(N1511:N1519))</f>
         <v/>
       </c>
       <c r="G1510" s="6">
-        <f>SUM(G1511:G1519)/SUM(N1511:N1519)</f>
+        <f>IF(SUM(N1511:N1519)=0,0,(SUM(G1511:G1519)/SUM(N1511:N1519))</f>
         <v/>
       </c>
       <c r="H1510" s="6">
-        <f>SUM(H1511:H1519)/SUM(N1511:N1519)</f>
+        <f>IF(SUM(N1511:N1519)=0,0,(SUM(H1511:H1519)/SUM(N1511:N1519))</f>
         <v/>
       </c>
       <c r="I1510" s="6">
-        <f>SUM(I1511:I1519)/SUM(N1511:N1519)</f>
+        <f>IF(SUM(N1511:N1519)=0,0,(SUM(I1511:I1519)/SUM(N1511:N1519))</f>
         <v/>
       </c>
       <c r="J1510" s="6">
-        <f>SUM(J1511:J1519)/SUM(N1511:N1519)</f>
+        <f>IF(SUM(N1511:N1519)=0,0,(SUM(J1511:J1519)/SUM(N1511:N1519))</f>
         <v/>
       </c>
       <c r="K1510" s="6">
-        <f>SUM(K1511:K1519)/SUM(N1511:N1519)</f>
+        <f>IF(SUM(N1511:N1519)=0,0,(SUM(K1511:K1519)/SUM(N1511:N1519))</f>
         <v/>
       </c>
       <c r="L1510" s="6">
-        <f>SUM(L1511:L1519)/SUM(N1511:N1519)</f>
+        <f>IF(SUM(N1511:N1519)=0,0,(SUM(L1511:L1519)/SUM(N1511:N1519))</f>
         <v/>
       </c>
       <c r="M1510" s="6">
-        <f>SUM(M1511:M1519)/SUM(N1511:N1519)</f>
+        <f>IF(SUM(N1511:N1519)=0,0,(SUM(M1511:M1519)/SUM(N1511:N1519))</f>
         <v/>
       </c>
     </row>
@@ -41310,27 +41310,27 @@
         <v>17</v>
       </c>
       <c r="C1522" s="6">
-        <f>SUM(C1523:C1531)/SUM(I1523:I1531)</f>
+        <f>IF(SUM(I1523:I1531)=0,0,(SUM(C1523:C1531)/SUM(I1523:I1531))</f>
         <v/>
       </c>
       <c r="D1522" s="6">
-        <f>SUM(D1523:D1531)/SUM(I1523:I1531)</f>
+        <f>IF(SUM(I1523:I1531)=0,0,(SUM(D1523:D1531)/SUM(I1523:I1531))</f>
         <v/>
       </c>
       <c r="E1522" s="6">
-        <f>SUM(E1523:E1531)/SUM(I1523:I1531)</f>
+        <f>IF(SUM(I1523:I1531)=0,0,(SUM(E1523:E1531)/SUM(I1523:I1531))</f>
         <v/>
       </c>
       <c r="F1522" s="6">
-        <f>SUM(F1523:F1531)/SUM(I1523:I1531)</f>
+        <f>IF(SUM(I1523:I1531)=0,0,(SUM(F1523:F1531)/SUM(I1523:I1531))</f>
         <v/>
       </c>
       <c r="G1522" s="6">
-        <f>SUM(G1523:G1531)/SUM(I1523:I1531)</f>
+        <f>IF(SUM(I1523:I1531)=0,0,(SUM(G1523:G1531)/SUM(I1523:I1531))</f>
         <v/>
       </c>
       <c r="H1522" s="6">
-        <f>SUM(H1523:H1531)/SUM(I1523:I1531)</f>
+        <f>IF(SUM(I1523:I1531)=0,0,(SUM(H1523:H1531)/SUM(I1523:I1531))</f>
         <v/>
       </c>
     </row>
@@ -41644,15 +41644,15 @@
         <v>17</v>
       </c>
       <c r="C1534" s="6">
-        <f>SUM(C1535:C1543)/SUM(F1535:F1543)</f>
+        <f>IF(SUM(F1535:F1543)=0,0,(SUM(C1535:C1543)/SUM(F1535:F1543))</f>
         <v/>
       </c>
       <c r="D1534" s="6">
-        <f>SUM(D1535:D1543)/SUM(F1535:F1543)</f>
+        <f>IF(SUM(F1535:F1543)=0,0,(SUM(D1535:D1543)/SUM(F1535:F1543))</f>
         <v/>
       </c>
       <c r="E1534" s="6">
-        <f>SUM(E1535:E1543)/SUM(F1535:F1543)</f>
+        <f>IF(SUM(F1535:F1543)=0,0,(SUM(E1535:E1543)/SUM(F1535:F1543))</f>
         <v/>
       </c>
     </row>
@@ -41899,31 +41899,31 @@
         <v>17</v>
       </c>
       <c r="C1552" s="6">
-        <f>SUM(C1553:C1564)/SUM(J1553:J1564)</f>
+        <f>IF(SUM(J1553:J1564)=0,0,(SUM(C1553:C1564)/SUM(J1553:J1564))</f>
         <v/>
       </c>
       <c r="D1552" s="6">
-        <f>SUM(D1553:D1564)/SUM(J1553:J1564)</f>
+        <f>IF(SUM(J1553:J1564)=0,0,(SUM(D1553:D1564)/SUM(J1553:J1564))</f>
         <v/>
       </c>
       <c r="E1552" s="6">
-        <f>SUM(E1553:E1564)/SUM(J1553:J1564)</f>
+        <f>IF(SUM(J1553:J1564)=0,0,(SUM(E1553:E1564)/SUM(J1553:J1564))</f>
         <v/>
       </c>
       <c r="F1552" s="6">
-        <f>SUM(F1553:F1564)/SUM(J1553:J1564)</f>
+        <f>IF(SUM(J1553:J1564)=0,0,(SUM(F1553:F1564)/SUM(J1553:J1564))</f>
         <v/>
       </c>
       <c r="G1552" s="6">
-        <f>SUM(G1553:G1564)/SUM(J1553:J1564)</f>
+        <f>IF(SUM(J1553:J1564)=0,0,(SUM(G1553:G1564)/SUM(J1553:J1564))</f>
         <v/>
       </c>
       <c r="H1552" s="6">
-        <f>SUM(H1553:H1564)/SUM(J1553:J1564)</f>
+        <f>IF(SUM(J1553:J1564)=0,0,(SUM(H1553:H1564)/SUM(J1553:J1564))</f>
         <v/>
       </c>
       <c r="I1552" s="6">
-        <f>SUM(I1553:I1564)/SUM(J1553:J1564)</f>
+        <f>IF(SUM(J1553:J1564)=0,0,(SUM(I1553:I1564)/SUM(J1553:J1564))</f>
         <v/>
       </c>
     </row>
@@ -42397,15 +42397,15 @@
         <v>17</v>
       </c>
       <c r="C1567" s="6">
-        <f>SUM(C1568:C1579)/SUM(F1568:F1579)</f>
+        <f>IF(SUM(F1568:F1579)=0,0,(SUM(C1568:C1579)/SUM(F1568:F1579))</f>
         <v/>
       </c>
       <c r="D1567" s="6">
-        <f>SUM(D1568:D1579)/SUM(F1568:F1579)</f>
+        <f>IF(SUM(F1568:F1579)=0,0,(SUM(D1568:D1579)/SUM(F1568:F1579))</f>
         <v/>
       </c>
       <c r="E1567" s="6">
-        <f>SUM(E1568:E1579)/SUM(F1568:F1579)</f>
+        <f>IF(SUM(F1568:F1579)=0,0,(SUM(E1568:E1579)/SUM(F1568:F1579))</f>
         <v/>
       </c>
     </row>
@@ -42710,15 +42710,15 @@
         <v>17</v>
       </c>
       <c r="C1582" s="6">
-        <f>SUM(C1583:C1594)/SUM(F1583:F1594)</f>
+        <f>IF(SUM(F1583:F1594)=0,0,(SUM(C1583:C1594)/SUM(F1583:F1594))</f>
         <v/>
       </c>
       <c r="D1582" s="6">
-        <f>SUM(D1583:D1594)/SUM(F1583:F1594)</f>
+        <f>IF(SUM(F1583:F1594)=0,0,(SUM(D1583:D1594)/SUM(F1583:F1594))</f>
         <v/>
       </c>
       <c r="E1582" s="6">
-        <f>SUM(E1583:E1594)/SUM(F1583:F1594)</f>
+        <f>IF(SUM(F1583:F1594)=0,0,(SUM(E1583:E1594)/SUM(F1583:F1594))</f>
         <v/>
       </c>
     </row>
@@ -43025,19 +43025,19 @@
         <v>17</v>
       </c>
       <c r="C1603" s="6">
-        <f>SUM(C1604:C1605)/SUM(G1604:G1605)</f>
+        <f>IF(SUM(G1604:G1605)=0,0,(SUM(C1604:C1605)/SUM(G1604:G1605))</f>
         <v/>
       </c>
       <c r="D1603" s="6">
-        <f>SUM(D1604:D1605)/SUM(G1604:G1605)</f>
+        <f>IF(SUM(G1604:G1605)=0,0,(SUM(D1604:D1605)/SUM(G1604:G1605))</f>
         <v/>
       </c>
       <c r="E1603" s="6">
-        <f>SUM(E1604:E1605)/SUM(G1604:G1605)</f>
+        <f>IF(SUM(G1604:G1605)=0,0,(SUM(E1604:E1605)/SUM(G1604:G1605))</f>
         <v/>
       </c>
       <c r="F1603" s="6">
-        <f>SUM(F1604:F1605)/SUM(G1604:G1605)</f>
+        <f>IF(SUM(G1604:G1605)=0,0,(SUM(F1604:F1605)/SUM(G1604:G1605))</f>
         <v/>
       </c>
     </row>
@@ -43118,11 +43118,11 @@
         <v>17</v>
       </c>
       <c r="C1608" s="6">
-        <f>SUM(C1609:C1610)/SUM(E1609:E1610)</f>
+        <f>IF(SUM(E1609:E1610)=0,0,(SUM(C1609:C1610)/SUM(E1609:E1610))</f>
         <v/>
       </c>
       <c r="D1608" s="6">
-        <f>SUM(D1609:D1610)/SUM(E1609:E1610)</f>
+        <f>IF(SUM(E1609:E1610)=0,0,(SUM(D1609:D1610)/SUM(E1609:E1610))</f>
         <v/>
       </c>
     </row>
@@ -43188,11 +43188,11 @@
         <v>17</v>
       </c>
       <c r="C1613" s="6">
-        <f>SUM(C1614:C1615)/SUM(E1614:E1615)</f>
+        <f>IF(SUM(E1614:E1615)=0,0,(SUM(C1614:C1615)/SUM(E1614:E1615))</f>
         <v/>
       </c>
       <c r="D1613" s="6">
-        <f>SUM(D1614:D1615)/SUM(E1614:E1615)</f>
+        <f>IF(SUM(E1614:E1615)=0,0,(SUM(D1614:D1615)/SUM(E1614:E1615))</f>
         <v/>
       </c>
     </row>
@@ -43268,19 +43268,19 @@
         <v>17</v>
       </c>
       <c r="C1624" s="6">
-        <f>SUM(C1625:C1626)/SUM(G1625:G1626)</f>
+        <f>IF(SUM(G1625:G1626)=0,0,(SUM(C1625:C1626)/SUM(G1625:G1626))</f>
         <v/>
       </c>
       <c r="D1624" s="6">
-        <f>SUM(D1625:D1626)/SUM(G1625:G1626)</f>
+        <f>IF(SUM(G1625:G1626)=0,0,(SUM(D1625:D1626)/SUM(G1625:G1626))</f>
         <v/>
       </c>
       <c r="E1624" s="6">
-        <f>SUM(E1625:E1626)/SUM(G1625:G1626)</f>
+        <f>IF(SUM(G1625:G1626)=0,0,(SUM(E1625:E1626)/SUM(G1625:G1626))</f>
         <v/>
       </c>
       <c r="F1624" s="6">
-        <f>SUM(F1625:F1626)/SUM(G1625:G1626)</f>
+        <f>IF(SUM(G1625:G1626)=0,0,(SUM(F1625:F1626)/SUM(G1625:G1626))</f>
         <v/>
       </c>
     </row>
@@ -43368,19 +43368,19 @@
         <v>17</v>
       </c>
       <c r="C1629" s="6">
-        <f>SUM(C1630:C1631)/SUM(G1630:G1631)</f>
+        <f>IF(SUM(G1630:G1631)=0,0,(SUM(C1630:C1631)/SUM(G1630:G1631))</f>
         <v/>
       </c>
       <c r="D1629" s="6">
-        <f>SUM(D1630:D1631)/SUM(G1630:G1631)</f>
+        <f>IF(SUM(G1630:G1631)=0,0,(SUM(D1630:D1631)/SUM(G1630:G1631))</f>
         <v/>
       </c>
       <c r="E1629" s="6">
-        <f>SUM(E1630:E1631)/SUM(G1630:G1631)</f>
+        <f>IF(SUM(G1630:G1631)=0,0,(SUM(E1630:E1631)/SUM(G1630:G1631))</f>
         <v/>
       </c>
       <c r="F1629" s="6">
-        <f>SUM(F1630:F1631)/SUM(G1630:G1631)</f>
+        <f>IF(SUM(G1630:G1631)=0,0,(SUM(F1630:F1631)/SUM(G1630:G1631))</f>
         <v/>
       </c>
     </row>
@@ -43458,11 +43458,11 @@
         <v>17</v>
       </c>
       <c r="C1634" s="6">
-        <f>SUM(C1635:C1636)/SUM(E1635:E1636)</f>
+        <f>IF(SUM(E1635:E1636)=0,0,(SUM(C1635:C1636)/SUM(E1635:E1636))</f>
         <v/>
       </c>
       <c r="D1634" s="6">
-        <f>SUM(D1635:D1636)/SUM(E1635:E1636)</f>
+        <f>IF(SUM(E1635:E1636)=0,0,(SUM(D1635:D1636)/SUM(E1635:E1636))</f>
         <v/>
       </c>
     </row>
@@ -43552,39 +43552,39 @@
         <v>17</v>
       </c>
       <c r="C1645" s="6">
-        <f>SUM(C1646:C1653)/SUM(L1646:L1653)</f>
+        <f>IF(SUM(L1646:L1653)=0,0,(SUM(C1646:C1653)/SUM(L1646:L1653))</f>
         <v/>
       </c>
       <c r="D1645" s="6">
-        <f>SUM(D1646:D1653)/SUM(L1646:L1653)</f>
+        <f>IF(SUM(L1646:L1653)=0,0,(SUM(D1646:D1653)/SUM(L1646:L1653))</f>
         <v/>
       </c>
       <c r="E1645" s="6">
-        <f>SUM(E1646:E1653)/SUM(L1646:L1653)</f>
+        <f>IF(SUM(L1646:L1653)=0,0,(SUM(E1646:E1653)/SUM(L1646:L1653))</f>
         <v/>
       </c>
       <c r="F1645" s="6">
-        <f>SUM(F1646:F1653)/SUM(L1646:L1653)</f>
+        <f>IF(SUM(L1646:L1653)=0,0,(SUM(F1646:F1653)/SUM(L1646:L1653))</f>
         <v/>
       </c>
       <c r="G1645" s="6">
-        <f>SUM(G1646:G1653)/SUM(L1646:L1653)</f>
+        <f>IF(SUM(L1646:L1653)=0,0,(SUM(G1646:G1653)/SUM(L1646:L1653))</f>
         <v/>
       </c>
       <c r="H1645" s="6">
-        <f>SUM(H1646:H1653)/SUM(L1646:L1653)</f>
+        <f>IF(SUM(L1646:L1653)=0,0,(SUM(H1646:H1653)/SUM(L1646:L1653))</f>
         <v/>
       </c>
       <c r="I1645" s="6">
-        <f>SUM(I1646:I1653)/SUM(L1646:L1653)</f>
+        <f>IF(SUM(L1646:L1653)=0,0,(SUM(I1646:I1653)/SUM(L1646:L1653))</f>
         <v/>
       </c>
       <c r="J1645" s="6">
-        <f>SUM(J1646:J1653)/SUM(L1646:L1653)</f>
+        <f>IF(SUM(L1646:L1653)=0,0,(SUM(J1646:J1653)/SUM(L1646:L1653))</f>
         <v/>
       </c>
       <c r="K1645" s="6">
-        <f>SUM(K1646:K1653)/SUM(L1646:L1653)</f>
+        <f>IF(SUM(L1646:L1653)=0,0,(SUM(K1646:K1653)/SUM(L1646:L1653))</f>
         <v/>
       </c>
     </row>
@@ -43969,31 +43969,31 @@
         <v>17</v>
       </c>
       <c r="C1656" s="6">
-        <f>SUM(C1657:C1664)/SUM(J1657:J1664)</f>
+        <f>IF(SUM(J1657:J1664)=0,0,(SUM(C1657:C1664)/SUM(J1657:J1664))</f>
         <v/>
       </c>
       <c r="D1656" s="6">
-        <f>SUM(D1657:D1664)/SUM(J1657:J1664)</f>
+        <f>IF(SUM(J1657:J1664)=0,0,(SUM(D1657:D1664)/SUM(J1657:J1664))</f>
         <v/>
       </c>
       <c r="E1656" s="6">
-        <f>SUM(E1657:E1664)/SUM(J1657:J1664)</f>
+        <f>IF(SUM(J1657:J1664)=0,0,(SUM(E1657:E1664)/SUM(J1657:J1664))</f>
         <v/>
       </c>
       <c r="F1656" s="6">
-        <f>SUM(F1657:F1664)/SUM(J1657:J1664)</f>
+        <f>IF(SUM(J1657:J1664)=0,0,(SUM(F1657:F1664)/SUM(J1657:J1664))</f>
         <v/>
       </c>
       <c r="G1656" s="6">
-        <f>SUM(G1657:G1664)/SUM(J1657:J1664)</f>
+        <f>IF(SUM(J1657:J1664)=0,0,(SUM(G1657:G1664)/SUM(J1657:J1664))</f>
         <v/>
       </c>
       <c r="H1656" s="6">
-        <f>SUM(H1657:H1664)/SUM(J1657:J1664)</f>
+        <f>IF(SUM(J1657:J1664)=0,0,(SUM(H1657:H1664)/SUM(J1657:J1664))</f>
         <v/>
       </c>
       <c r="I1656" s="6">
-        <f>SUM(I1657:I1664)/SUM(J1657:J1664)</f>
+        <f>IF(SUM(J1657:J1664)=0,0,(SUM(I1657:I1664)/SUM(J1657:J1664))</f>
         <v/>
       </c>
     </row>
@@ -44295,11 +44295,11 @@
         <v>17</v>
       </c>
       <c r="C1667" s="6">
-        <f>SUM(C1668:C1675)/SUM(E1668:E1675)</f>
+        <f>IF(SUM(E1668:E1675)=0,0,(SUM(C1668:C1675)/SUM(E1668:E1675))</f>
         <v/>
       </c>
       <c r="D1667" s="6">
-        <f>SUM(D1668:D1675)/SUM(E1668:E1675)</f>
+        <f>IF(SUM(E1668:E1675)=0,0,(SUM(D1668:D1675)/SUM(E1668:E1675))</f>
         <v/>
       </c>
     </row>
@@ -44493,23 +44493,23 @@
         <v>17</v>
       </c>
       <c r="C1684" s="6">
-        <f>SUM(C1685:C1688)/SUM(H1685:H1688)</f>
+        <f>IF(SUM(H1685:H1688)=0,0,(SUM(C1685:C1688)/SUM(H1685:H1688))</f>
         <v/>
       </c>
       <c r="D1684" s="6">
-        <f>SUM(D1685:D1688)/SUM(H1685:H1688)</f>
+        <f>IF(SUM(H1685:H1688)=0,0,(SUM(D1685:D1688)/SUM(H1685:H1688))</f>
         <v/>
       </c>
       <c r="E1684" s="6">
-        <f>SUM(E1685:E1688)/SUM(H1685:H1688)</f>
+        <f>IF(SUM(H1685:H1688)=0,0,(SUM(E1685:E1688)/SUM(H1685:H1688))</f>
         <v/>
       </c>
       <c r="F1684" s="6">
-        <f>SUM(F1685:F1688)/SUM(H1685:H1688)</f>
+        <f>IF(SUM(H1685:H1688)=0,0,(SUM(F1685:F1688)/SUM(H1685:H1688))</f>
         <v/>
       </c>
       <c r="G1684" s="6">
-        <f>SUM(G1685:G1688)/SUM(H1685:H1688)</f>
+        <f>IF(SUM(H1685:H1688)=0,0,(SUM(G1685:G1688)/SUM(H1685:H1688))</f>
         <v/>
       </c>
     </row>
@@ -44662,15 +44662,15 @@
         <v>17</v>
       </c>
       <c r="C1691" s="6">
-        <f>SUM(C1692:C1695)/SUM(F1692:F1695)</f>
+        <f>IF(SUM(F1692:F1695)=0,0,(SUM(C1692:C1695)/SUM(F1692:F1695))</f>
         <v/>
       </c>
       <c r="D1691" s="6">
-        <f>SUM(D1692:D1695)/SUM(F1692:F1695)</f>
+        <f>IF(SUM(F1692:F1695)=0,0,(SUM(D1692:D1695)/SUM(F1692:F1695))</f>
         <v/>
       </c>
       <c r="E1691" s="6">
-        <f>SUM(E1692:E1695)/SUM(F1692:F1695)</f>
+        <f>IF(SUM(F1692:F1695)=0,0,(SUM(E1692:E1695)/SUM(F1692:F1695))</f>
         <v/>
       </c>
     </row>
@@ -44788,11 +44788,11 @@
         <v>17</v>
       </c>
       <c r="C1698" s="6">
-        <f>SUM(C1699:C1702)/SUM(E1699:E1702)</f>
+        <f>IF(SUM(E1699:E1702)=0,0,(SUM(C1699:C1702)/SUM(E1699:E1702))</f>
         <v/>
       </c>
       <c r="D1698" s="6">
-        <f>SUM(D1699:D1702)/SUM(E1699:E1702)</f>
+        <f>IF(SUM(E1699:E1702)=0,0,(SUM(D1699:D1702)/SUM(E1699:E1702))</f>
         <v/>
       </c>
     </row>
@@ -44920,35 +44920,35 @@
         <v>17</v>
       </c>
       <c r="C1711" s="6">
-        <f>SUM(C1712:C1717)/SUM(K1712:K1717)</f>
+        <f>IF(SUM(K1712:K1717)=0,0,(SUM(C1712:C1717)/SUM(K1712:K1717))</f>
         <v/>
       </c>
       <c r="D1711" s="6">
-        <f>SUM(D1712:D1717)/SUM(K1712:K1717)</f>
+        <f>IF(SUM(K1712:K1717)=0,0,(SUM(D1712:D1717)/SUM(K1712:K1717))</f>
         <v/>
       </c>
       <c r="E1711" s="6">
-        <f>SUM(E1712:E1717)/SUM(K1712:K1717)</f>
+        <f>IF(SUM(K1712:K1717)=0,0,(SUM(E1712:E1717)/SUM(K1712:K1717))</f>
         <v/>
       </c>
       <c r="F1711" s="6">
-        <f>SUM(F1712:F1717)/SUM(K1712:K1717)</f>
+        <f>IF(SUM(K1712:K1717)=0,0,(SUM(F1712:F1717)/SUM(K1712:K1717))</f>
         <v/>
       </c>
       <c r="G1711" s="6">
-        <f>SUM(G1712:G1717)/SUM(K1712:K1717)</f>
+        <f>IF(SUM(K1712:K1717)=0,0,(SUM(G1712:G1717)/SUM(K1712:K1717))</f>
         <v/>
       </c>
       <c r="H1711" s="6">
-        <f>SUM(H1712:H1717)/SUM(K1712:K1717)</f>
+        <f>IF(SUM(K1712:K1717)=0,0,(SUM(H1712:H1717)/SUM(K1712:K1717))</f>
         <v/>
       </c>
       <c r="I1711" s="6">
-        <f>SUM(I1712:I1717)/SUM(K1712:K1717)</f>
+        <f>IF(SUM(K1712:K1717)=0,0,(SUM(I1712:I1717)/SUM(K1712:K1717))</f>
         <v/>
       </c>
       <c r="J1711" s="6">
-        <f>SUM(J1712:J1717)/SUM(K1712:K1717)</f>
+        <f>IF(SUM(K1712:K1717)=0,0,(SUM(J1712:J1717)/SUM(K1712:K1717))</f>
         <v/>
       </c>
     </row>
@@ -45218,15 +45218,15 @@
         <v>17</v>
       </c>
       <c r="C1720" s="6">
-        <f>SUM(C1721:C1726)/SUM(F1721:F1726)</f>
+        <f>IF(SUM(F1721:F1726)=0,0,(SUM(C1721:C1726)/SUM(F1721:F1726))</f>
         <v/>
       </c>
       <c r="D1720" s="6">
-        <f>SUM(D1721:D1726)/SUM(F1721:F1726)</f>
+        <f>IF(SUM(F1721:F1726)=0,0,(SUM(D1721:D1726)/SUM(F1721:F1726))</f>
         <v/>
       </c>
       <c r="E1720" s="6">
-        <f>SUM(E1721:E1726)/SUM(F1721:F1726)</f>
+        <f>IF(SUM(F1721:F1726)=0,0,(SUM(E1721:E1726)/SUM(F1721:F1726))</f>
         <v/>
       </c>
     </row>
@@ -45385,7 +45385,7 @@
         <v>17</v>
       </c>
       <c r="C1729" s="6">
-        <f>SUM(C1730:C1735)/SUM(D1730:D1735)</f>
+        <f>IF(SUM(D1730:D1735)=0,0,(SUM(C1730:C1735)/SUM(D1730:D1735))</f>
         <v/>
       </c>
     </row>

</xml_diff>